<commit_message>
added code to account for new 5th subject tag column added by tara/daniel
</commit_message>
<xml_diff>
--- a/saved_versions/fcheck_temp.xlsx
+++ b/saved_versions/fcheck_temp.xlsx
@@ -527,7 +527,7 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t xml:space="preserve">E POPULARITY  </t>
+          <t xml:space="preserve">E POPULARITY   </t>
         </is>
       </c>
     </row>
@@ -600,7 +600,7 @@
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t xml:space="preserve">TRADE ECONOMY  </t>
+          <t xml:space="preserve">TRADE ECONOMY   </t>
         </is>
       </c>
     </row>
@@ -668,7 +668,7 @@
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t xml:space="preserve">ENVIRONMENT   </t>
+          <t xml:space="preserve">ENVIRONMENT    </t>
         </is>
       </c>
     </row>
@@ -737,7 +737,7 @@
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t xml:space="preserve">ENVIRONMENT   </t>
+          <t xml:space="preserve">ENVIRONMENT    </t>
         </is>
       </c>
     </row>
@@ -811,7 +811,7 @@
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t xml:space="preserve">HEALTH CARE   </t>
+          <t xml:space="preserve">HEALTH CARE    </t>
         </is>
       </c>
     </row>
@@ -884,7 +884,7 @@
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t xml:space="preserve">HEALTH CARE   </t>
+          <t xml:space="preserve">HEALTH CARE    </t>
         </is>
       </c>
     </row>
@@ -962,7 +962,7 @@
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t xml:space="preserve">UNEMPLOYMENT ECONOMY WOMEN </t>
+          <t xml:space="preserve">UNEMPLOYMENT ECONOMY WOMEN  </t>
         </is>
       </c>
     </row>
@@ -1040,7 +1040,7 @@
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t xml:space="preserve">TRADE CHINA ECONOMY </t>
+          <t xml:space="preserve">TRADE CHINA ECONOMY  </t>
         </is>
       </c>
     </row>
@@ -1108,7 +1108,7 @@
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t xml:space="preserve">CENSUS   </t>
+          <t xml:space="preserve">CENSUS    </t>
         </is>
       </c>
     </row>
@@ -1192,7 +1192,7 @@
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>HILLARY CLINTON THE WALL DEMOCRATS IMMIGRATION</t>
+          <t xml:space="preserve">HILLARY CLINTON THE WALL DEMOCRATS IMMIGRATION </t>
         </is>
       </c>
     </row>
@@ -1265,7 +1265,7 @@
       </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t xml:space="preserve">DEMOCRATS IMMIGRATION  </t>
+          <t xml:space="preserve">DEMOCRATS IMMIGRATION   </t>
         </is>
       </c>
     </row>
@@ -1333,7 +1333,7 @@
       </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t xml:space="preserve">CROWDS   </t>
+          <t xml:space="preserve">CROWDS    </t>
         </is>
       </c>
     </row>
@@ -1401,7 +1401,7 @@
       </c>
       <c r="T14" t="inlineStr">
         <is>
-          <t xml:space="preserve">CROWDS   </t>
+          <t xml:space="preserve">CROWDS    </t>
         </is>
       </c>
     </row>
@@ -1470,7 +1470,7 @@
       </c>
       <c r="T15" t="inlineStr">
         <is>
-          <t xml:space="preserve">SOCIAL MEDIA   </t>
+          <t xml:space="preserve">SOCIAL MEDIA    </t>
         </is>
       </c>
     </row>
@@ -1549,7 +1549,7 @@
       </c>
       <c r="T16" t="inlineStr">
         <is>
-          <t xml:space="preserve">TRADE ECONOMY  </t>
+          <t xml:space="preserve">TRADE ECONOMY   </t>
         </is>
       </c>
     </row>
@@ -1623,7 +1623,7 @@
       </c>
       <c r="T17" t="inlineStr">
         <is>
-          <t xml:space="preserve">ECONOMY   </t>
+          <t xml:space="preserve">ECONOMY    </t>
         </is>
       </c>
     </row>
@@ -1701,7 +1701,7 @@
       </c>
       <c r="T18" t="inlineStr">
         <is>
-          <t xml:space="preserve">JOBS ECONOMY  </t>
+          <t xml:space="preserve">JOBS ECONOMY   </t>
         </is>
       </c>
     </row>
@@ -1790,7 +1790,7 @@
       </c>
       <c r="T19" t="inlineStr">
         <is>
-          <t>JOBS ECONOMY MANUFACTURING BARACK OBAMA</t>
+          <t xml:space="preserve">JOBS ECONOMY MANUFACTURING BARACK OBAMA </t>
         </is>
       </c>
     </row>
@@ -1864,7 +1864,7 @@
       </c>
       <c r="T20" t="inlineStr">
         <is>
-          <t xml:space="preserve">ENERGY   </t>
+          <t xml:space="preserve">ENERGY    </t>
         </is>
       </c>
     </row>
@@ -1942,7 +1942,7 @@
       </c>
       <c r="T21" t="inlineStr">
         <is>
-          <t xml:space="preserve">TRADE CHINA  </t>
+          <t xml:space="preserve">TRADE CHINA   </t>
         </is>
       </c>
     </row>
@@ -2008,7 +2008,7 @@
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>Economy</t>
+          <t>ECONOMY</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
@@ -2035,7 +2035,7 @@
       </c>
       <c r="T22" t="inlineStr">
         <is>
-          <t>TRADE CHINA FARMERS TARIFFS</t>
+          <t>TRADE CHINA FARMERS TARIFFS ECONOMY</t>
         </is>
       </c>
     </row>
@@ -2127,7 +2127,7 @@
       </c>
       <c r="T23" t="inlineStr">
         <is>
-          <t>TRADE CHINA ECONOMY TARIFFS</t>
+          <t xml:space="preserve">TRADE CHINA ECONOMY TARIFFS </t>
         </is>
       </c>
     </row>
@@ -2192,7 +2192,7 @@
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>Democrats</t>
+          <t>DEMOCRATS</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
@@ -2219,7 +2219,7 @@
       </c>
       <c r="T24" t="inlineStr">
         <is>
-          <t>TRADE CHINA ECONOMY TARIFFS</t>
+          <t>TRADE CHINA ECONOMY TARIFFS DEMOCRATS</t>
         </is>
       </c>
     </row>
@@ -2307,7 +2307,7 @@
       </c>
       <c r="T25" t="inlineStr">
         <is>
-          <t>CHINA TARIFFS TRADE FARMERS</t>
+          <t xml:space="preserve">CHINA TARIFFS TRADE FARMERS </t>
         </is>
       </c>
     </row>
@@ -2390,7 +2390,7 @@
       </c>
       <c r="T26" t="inlineStr">
         <is>
-          <t xml:space="preserve">TRADE ECONOMY NAFTA AND USMCA </t>
+          <t xml:space="preserve">TRADE ECONOMY NAFTA AND USMCA  </t>
         </is>
       </c>
     </row>
@@ -2458,7 +2458,7 @@
       </c>
       <c r="T27" t="inlineStr">
         <is>
-          <t xml:space="preserve">CENSUS   </t>
+          <t xml:space="preserve">CENSUS    </t>
         </is>
       </c>
     </row>
@@ -2533,7 +2533,7 @@
       </c>
       <c r="T28" t="inlineStr">
         <is>
-          <t xml:space="preserve">MUELLER INVESTIGATION RUSSIA INVESTIGATION  </t>
+          <t xml:space="preserve">MUELLER INVESTIGATION RUSSIA INVESTIGATION   </t>
         </is>
       </c>
     </row>
@@ -2611,7 +2611,7 @@
       </c>
       <c r="T29" t="inlineStr">
         <is>
-          <t xml:space="preserve">IMMIGRATION MEXICO  </t>
+          <t xml:space="preserve">IMMIGRATION MEXICO   </t>
         </is>
       </c>
     </row>
@@ -2686,7 +2686,7 @@
       </c>
       <c r="T30" t="inlineStr">
         <is>
-          <t xml:space="preserve">IMMIGRATION MEDIA  </t>
+          <t xml:space="preserve">IMMIGRATION MEDIA   </t>
         </is>
       </c>
     </row>
@@ -2754,7 +2754,7 @@
       </c>
       <c r="T31" t="inlineStr">
         <is>
-          <t xml:space="preserve">PAST PRESIDENTS   </t>
+          <t xml:space="preserve">PAST PRESIDENTS    </t>
         </is>
       </c>
     </row>
@@ -2833,7 +2833,7 @@
       </c>
       <c r="T32" t="inlineStr">
         <is>
-          <t xml:space="preserve">VETERANS HEALTH CARE MILITARY </t>
+          <t xml:space="preserve">VETERANS HEALTH CARE MILITARY  </t>
         </is>
       </c>
     </row>
@@ -2919,7 +2919,7 @@
       </c>
       <c r="T33" t="inlineStr">
         <is>
-          <t>ECONOMY JAPAN GERMANY TRADE</t>
+          <t xml:space="preserve">ECONOMY JAPAN GERMANY TRADE </t>
         </is>
       </c>
     </row>
@@ -2993,7 +2993,7 @@
       </c>
       <c r="T34" t="inlineStr">
         <is>
-          <t xml:space="preserve">IRAN BARACK OBAMA DEMOCRATS </t>
+          <t xml:space="preserve">IRAN BARACK OBAMA DEMOCRATS  </t>
         </is>
       </c>
     </row>
@@ -3062,7 +3062,7 @@
       </c>
       <c r="T35" t="inlineStr">
         <is>
-          <t xml:space="preserve">THE SQUAD DEMOCRATS ISRAEL </t>
+          <t xml:space="preserve">THE SQUAD DEMOCRATS ISRAEL  </t>
         </is>
       </c>
     </row>
@@ -3131,7 +3131,7 @@
       </c>
       <c r="T36" t="inlineStr">
         <is>
-          <t xml:space="preserve">THE SQUAD DEMOCRATS ISRAEL </t>
+          <t xml:space="preserve">THE SQUAD DEMOCRATS ISRAEL  </t>
         </is>
       </c>
     </row>
@@ -3200,7 +3200,7 @@
       </c>
       <c r="T37" t="inlineStr">
         <is>
-          <t xml:space="preserve">THE SQUAD DEMOCRATS ISRAEL </t>
+          <t xml:space="preserve">THE SQUAD DEMOCRATS ISRAEL  </t>
         </is>
       </c>
     </row>
@@ -3275,7 +3275,7 @@
       </c>
       <c r="T38" t="inlineStr">
         <is>
-          <t xml:space="preserve">FARMERS   </t>
+          <t xml:space="preserve">FARMERS    </t>
         </is>
       </c>
     </row>
@@ -3359,7 +3359,7 @@
       </c>
       <c r="T39" t="inlineStr">
         <is>
-          <t xml:space="preserve">VETERANS HEALTH CARE MILITARY </t>
+          <t xml:space="preserve">VETERANS HEALTH CARE MILITARY  </t>
         </is>
       </c>
     </row>
@@ -3438,7 +3438,7 @@
       </c>
       <c r="T40" t="inlineStr">
         <is>
-          <t xml:space="preserve">IMMIGRATION CARAVAN DEMOCRATS </t>
+          <t xml:space="preserve">IMMIGRATION CARAVAN DEMOCRATS  </t>
         </is>
       </c>
     </row>
@@ -3511,7 +3511,7 @@
       </c>
       <c r="T41" t="inlineStr">
         <is>
-          <t xml:space="preserve">IMMIGRATION COURTS  </t>
+          <t xml:space="preserve">IMMIGRATION COURTS   </t>
         </is>
       </c>
     </row>
@@ -3591,7 +3591,7 @@
       </c>
       <c r="T42" t="inlineStr">
         <is>
-          <t xml:space="preserve">HUMAN TRAFFICKING DEMOCRATS IMMIGRATION </t>
+          <t xml:space="preserve">HUMAN TRAFFICKING DEMOCRATS IMMIGRATION  </t>
         </is>
       </c>
     </row>
@@ -3664,7 +3664,7 @@
       </c>
       <c r="T43" t="inlineStr">
         <is>
-          <t xml:space="preserve">IMMIGRATION DEMOCRATS  </t>
+          <t xml:space="preserve">IMMIGRATION DEMOCRATS   </t>
         </is>
       </c>
     </row>
@@ -3733,7 +3733,7 @@
       </c>
       <c r="T44" t="inlineStr">
         <is>
-          <t xml:space="preserve">ENERGY   </t>
+          <t xml:space="preserve">ENERGY    </t>
         </is>
       </c>
     </row>
@@ -3812,7 +3812,7 @@
       </c>
       <c r="T45" t="inlineStr">
         <is>
-          <t xml:space="preserve">NORTH KOREA VETERANS MILITARY </t>
+          <t xml:space="preserve">NORTH KOREA VETERANS MILITARY  </t>
         </is>
       </c>
     </row>
@@ -3890,7 +3890,7 @@
       </c>
       <c r="T46" t="inlineStr">
         <is>
-          <t xml:space="preserve">TRADE MEXICO NAFTA AND USMCA </t>
+          <t xml:space="preserve">TRADE MEXICO NAFTA AND USMCA  </t>
         </is>
       </c>
     </row>
@@ -3964,7 +3964,7 @@
       </c>
       <c r="T47" t="inlineStr">
         <is>
-          <t xml:space="preserve">WALL IMMIGRATION  </t>
+          <t xml:space="preserve">WALL IMMIGRATION   </t>
         </is>
       </c>
     </row>
@@ -4042,7 +4042,7 @@
       </c>
       <c r="T48" t="inlineStr">
         <is>
-          <t xml:space="preserve">ECONOMY WOMEN UNEMPLOYMENT </t>
+          <t xml:space="preserve">ECONOMY WOMEN UNEMPLOYMENT  </t>
         </is>
       </c>
     </row>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="T49" t="inlineStr">
         <is>
-          <t>CHINA TARIFFS TRADE FARMERS</t>
+          <t xml:space="preserve">CHINA TARIFFS TRADE FARMERS </t>
         </is>
       </c>
     </row>
@@ -4181,7 +4181,7 @@
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>t</t>
+          <t>T</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
@@ -4208,7 +4208,7 @@
       </c>
       <c r="T50" t="inlineStr">
         <is>
-          <t xml:space="preserve">CHINA ECONOMY TRADE </t>
+          <t>CHINA ECONOMY TRADE  T</t>
         </is>
       </c>
     </row>
@@ -4281,7 +4281,7 @@
       </c>
       <c r="T51" t="inlineStr">
         <is>
-          <t xml:space="preserve">CHINA ECONOMY  </t>
+          <t xml:space="preserve">CHINA ECONOMY   </t>
         </is>
       </c>
     </row>
@@ -4362,7 +4362,7 @@
       </c>
       <c r="T52" t="inlineStr">
         <is>
-          <t xml:space="preserve">IRAN BARACK OBAMA DEMOCRATS </t>
+          <t xml:space="preserve">IRAN BARACK OBAMA DEMOCRATS  </t>
         </is>
       </c>
     </row>
@@ -4437,7 +4437,7 @@
       </c>
       <c r="T53" t="inlineStr">
         <is>
-          <t xml:space="preserve">STOCK MARKET ECONOMY  </t>
+          <t xml:space="preserve">STOCK MARKET ECONOMY   </t>
         </is>
       </c>
     </row>
@@ -4522,7 +4522,7 @@
       </c>
       <c r="T54" t="inlineStr">
         <is>
-          <t xml:space="preserve">THE SQUAD TERRORISM DEMOCRATS </t>
+          <t xml:space="preserve">THE SQUAD TERRORISM DEMOCRATS  </t>
         </is>
       </c>
     </row>
@@ -4604,7 +4604,7 @@
       </c>
       <c r="T55" t="inlineStr">
         <is>
-          <t xml:space="preserve">THE SQUAD POLLS DEMOCRATS </t>
+          <t xml:space="preserve">THE SQUAD POLLS DEMOCRATS  </t>
         </is>
       </c>
     </row>
@@ -4674,7 +4674,7 @@
       </c>
       <c r="T56" t="inlineStr">
         <is>
-          <t xml:space="preserve">IRAN   </t>
+          <t xml:space="preserve">IRAN    </t>
         </is>
       </c>
     </row>
@@ -4751,7 +4751,7 @@
       </c>
       <c r="T57" t="inlineStr">
         <is>
-          <t xml:space="preserve">IMMIGRATION DEMOCRATS  </t>
+          <t xml:space="preserve">IMMIGRATION DEMOCRATS   </t>
         </is>
       </c>
     </row>
@@ -4824,7 +4824,7 @@
       </c>
       <c r="T58" t="inlineStr">
         <is>
-          <t xml:space="preserve">CROWDS   </t>
+          <t xml:space="preserve">CROWDS    </t>
         </is>
       </c>
     </row>
@@ -4902,7 +4902,7 @@
       </c>
       <c r="T59" t="inlineStr">
         <is>
-          <t xml:space="preserve">HEALTH CARE DEMOCRATS  </t>
+          <t xml:space="preserve">HEALTH CARE DEMOCRATS   </t>
         </is>
       </c>
     </row>
@@ -4984,7 +4984,7 @@
       </c>
       <c r="T60" t="inlineStr">
         <is>
-          <t xml:space="preserve">THE SQUAD DEMOCRATS TERRORISM </t>
+          <t xml:space="preserve">THE SQUAD DEMOCRATS TERRORISM  </t>
         </is>
       </c>
     </row>
@@ -5068,7 +5068,7 @@
       </c>
       <c r="T61" t="inlineStr">
         <is>
-          <t xml:space="preserve">IMMIGRATION HISPANICS THE WALL </t>
+          <t xml:space="preserve">IMMIGRATION HISPANICS THE WALL  </t>
         </is>
       </c>
     </row>
@@ -5157,7 +5157,7 @@
       </c>
       <c r="T62" t="inlineStr">
         <is>
-          <t>IMMIGRATION DEMOCRATS HEALTH CARE CALIFORNIA</t>
+          <t xml:space="preserve">IMMIGRATION DEMOCRATS HEALTH CARE CALIFORNIA </t>
         </is>
       </c>
     </row>
@@ -5237,7 +5237,7 @@
       </c>
       <c r="T63" t="inlineStr">
         <is>
-          <t xml:space="preserve">HUMAN TRAFFICKING IMMIGRATION  </t>
+          <t xml:space="preserve">HUMAN TRAFFICKING IMMIGRATION   </t>
         </is>
       </c>
     </row>
@@ -5322,7 +5322,7 @@
       </c>
       <c r="T64" t="inlineStr">
         <is>
-          <t xml:space="preserve">HUMAN TRAFFICKING DEMOCRATS IMMIGRATION </t>
+          <t xml:space="preserve">HUMAN TRAFFICKING DEMOCRATS IMMIGRATION  </t>
         </is>
       </c>
     </row>
@@ -5402,7 +5402,7 @@
       </c>
       <c r="T65" t="inlineStr">
         <is>
-          <t xml:space="preserve">WALL DEMOCRATS  </t>
+          <t xml:space="preserve">WALL DEMOCRATS   </t>
         </is>
       </c>
     </row>
@@ -5481,7 +5481,7 @@
       </c>
       <c r="T66" t="inlineStr">
         <is>
-          <t xml:space="preserve">DEMOCRATS IMMIGRATION GUNS </t>
+          <t xml:space="preserve">DEMOCRATS IMMIGRATION GUNS  </t>
         </is>
       </c>
     </row>
@@ -5565,7 +5565,7 @@
       </c>
       <c r="T67" t="inlineStr">
         <is>
-          <t xml:space="preserve">IMMIGRATION DEMOCRATS MEDIA </t>
+          <t xml:space="preserve">IMMIGRATION DEMOCRATS MEDIA  </t>
         </is>
       </c>
     </row>
@@ -5644,7 +5644,7 @@
       </c>
       <c r="T68" t="inlineStr">
         <is>
-          <t xml:space="preserve">ECONOMY UNEMPLOYMENT  </t>
+          <t xml:space="preserve">ECONOMY UNEMPLOYMENT   </t>
         </is>
       </c>
     </row>
@@ -5728,7 +5728,7 @@
       </c>
       <c r="T69" t="inlineStr">
         <is>
-          <t xml:space="preserve">ECONOMY NORTH CAROLINA UNEMPLOYMENT </t>
+          <t xml:space="preserve">ECONOMY NORTH CAROLINA UNEMPLOYMENT  </t>
         </is>
       </c>
     </row>
@@ -5806,7 +5806,7 @@
       </c>
       <c r="T70" t="inlineStr">
         <is>
-          <t xml:space="preserve">POLLS 2016 ELECTION  </t>
+          <t xml:space="preserve">POLLS 2016 ELECTION   </t>
         </is>
       </c>
     </row>
@@ -5896,7 +5896,7 @@
       </c>
       <c r="T71" t="inlineStr">
         <is>
-          <t>POLLS 2016 ELECTION DEMOCRATS HILLARY CLINTON</t>
+          <t xml:space="preserve">POLLS 2016 ELECTION DEMOCRATS HILLARY CLINTON </t>
         </is>
       </c>
     </row>
@@ -5980,7 +5980,7 @@
       </c>
       <c r="T72" t="inlineStr">
         <is>
-          <t xml:space="preserve">NATO MILITARY EUROPE </t>
+          <t xml:space="preserve">NATO MILITARY EUROPE  </t>
         </is>
       </c>
     </row>
@@ -6063,7 +6063,7 @@
       </c>
       <c r="T73" t="inlineStr">
         <is>
-          <t xml:space="preserve">TRADE CHINA EUROPE </t>
+          <t xml:space="preserve">TRADE CHINA EUROPE  </t>
         </is>
       </c>
     </row>
@@ -6151,7 +6151,7 @@
       </c>
       <c r="T74" t="inlineStr">
         <is>
-          <t>2020 ELECTION 2020 DEMOCRATIC CANDIDATES DEMOCRATS ELIZABETH WARREN</t>
+          <t xml:space="preserve">2020 ELECTION 2020 DEMOCRATIC CANDIDATES DEMOCRATS ELIZABETH WARREN </t>
         </is>
       </c>
     </row>
@@ -6234,7 +6234,7 @@
       </c>
       <c r="T75" t="inlineStr">
         <is>
-          <t xml:space="preserve">MILITARY HEALTH CARE VETERANS </t>
+          <t xml:space="preserve">MILITARY HEALTH CARE VETERANS  </t>
         </is>
       </c>
     </row>
@@ -6319,7 +6319,7 @@
       </c>
       <c r="T76" t="inlineStr">
         <is>
-          <t xml:space="preserve">PRESCRIPTION DRUGS DEMOCRATS HEALTH CARE </t>
+          <t xml:space="preserve">PRESCRIPTION DRUGS DEMOCRATS HEALTH CARE  </t>
         </is>
       </c>
     </row>
@@ -6392,7 +6392,7 @@
       </c>
       <c r="T77" t="inlineStr">
         <is>
-          <t xml:space="preserve">OPIOD EPIDEMIC   </t>
+          <t xml:space="preserve">OPIOD EPIDEMIC    </t>
         </is>
       </c>
     </row>
@@ -6475,7 +6475,7 @@
       </c>
       <c r="T78" t="inlineStr">
         <is>
-          <t xml:space="preserve">ECONOMY WOMEN UNEMPLOYMENT </t>
+          <t xml:space="preserve">ECONOMY WOMEN UNEMPLOYMENT  </t>
         </is>
       </c>
     </row>
@@ -6556,7 +6556,7 @@
       </c>
       <c r="T79" t="inlineStr">
         <is>
-          <t xml:space="preserve">MUELLER INVESTIGATION OBSTRUCTION OF JUSTICE  </t>
+          <t xml:space="preserve">MUELLER INVESTIGATION OBSTRUCTION OF JUSTICE   </t>
         </is>
       </c>
     </row>
@@ -6630,7 +6630,7 @@
       </c>
       <c r="T80" t="inlineStr">
         <is>
-          <t xml:space="preserve">DEBT DEMOCRATS  </t>
+          <t xml:space="preserve">DEBT DEMOCRATS   </t>
         </is>
       </c>
     </row>
@@ -6704,7 +6704,7 @@
       </c>
       <c r="T81" t="inlineStr">
         <is>
-          <t xml:space="preserve">THE SQUAD CROWDS  </t>
+          <t xml:space="preserve">THE SQUAD CROWDS   </t>
         </is>
       </c>
     </row>
@@ -6783,7 +6783,7 @@
       </c>
       <c r="T82" t="inlineStr">
         <is>
-          <t xml:space="preserve">IRAN BARACK OBAMA  </t>
+          <t xml:space="preserve">IRAN BARACK OBAMA   </t>
         </is>
       </c>
     </row>
@@ -6857,7 +6857,7 @@
       </c>
       <c r="T83" t="inlineStr">
         <is>
-          <t xml:space="preserve">AMAZON MILITARY  </t>
+          <t xml:space="preserve">AMAZON MILITARY   </t>
         </is>
       </c>
     </row>
@@ -6932,7 +6932,7 @@
       </c>
       <c r="T84" t="inlineStr">
         <is>
-          <t xml:space="preserve">STEEL ECONOMY  </t>
+          <t xml:space="preserve">STEEL ECONOMY   </t>
         </is>
       </c>
     </row>
@@ -7002,7 +7002,7 @@
       </c>
       <c r="T85" t="inlineStr">
         <is>
-          <t xml:space="preserve">PUERTO RICO CONGRESS  </t>
+          <t xml:space="preserve">PUERTO RICO CONGRESS   </t>
         </is>
       </c>
     </row>
@@ -7073,7 +7073,7 @@
       </c>
       <c r="T86" t="inlineStr">
         <is>
-          <t xml:space="preserve">TERRORISM PAKISTAN  </t>
+          <t xml:space="preserve">TERRORISM PAKISTAN   </t>
         </is>
       </c>
     </row>
@@ -7150,7 +7150,7 @@
       </c>
       <c r="T87" t="inlineStr">
         <is>
-          <t xml:space="preserve">THE SQUAD POLLS DEMOCRATS </t>
+          <t xml:space="preserve">THE SQUAD POLLS DEMOCRATS  </t>
         </is>
       </c>
     </row>
@@ -7217,7 +7217,7 @@
       </c>
       <c r="T88" t="inlineStr">
         <is>
-          <t xml:space="preserve">DEMOCRATS IMMIGRATION  </t>
+          <t xml:space="preserve">DEMOCRATS IMMIGRATION   </t>
         </is>
       </c>
     </row>
@@ -7291,7 +7291,7 @@
       </c>
       <c r="T89" t="inlineStr">
         <is>
-          <t xml:space="preserve">CHINA TARIFFS TRADE </t>
+          <t xml:space="preserve">CHINA TARIFFS TRADE  </t>
         </is>
       </c>
     </row>
@@ -7365,7 +7365,7 @@
       </c>
       <c r="T90" t="inlineStr">
         <is>
-          <t xml:space="preserve">THE SQUAD DEMOCRATS  </t>
+          <t xml:space="preserve">THE SQUAD DEMOCRATS   </t>
         </is>
       </c>
     </row>
@@ -7435,7 +7435,7 @@
       </c>
       <c r="T91" t="inlineStr">
         <is>
-          <t xml:space="preserve">POLLS POPULARITY  </t>
+          <t xml:space="preserve">POLLS POPULARITY   </t>
         </is>
       </c>
     </row>
@@ -7511,7 +7511,7 @@
       </c>
       <c r="T92" t="inlineStr">
         <is>
-          <t xml:space="preserve">BARACK OBAMA DEBT  </t>
+          <t xml:space="preserve">BARACK OBAMA DEBT   </t>
         </is>
       </c>
     </row>
@@ -7592,7 +7592,7 @@
       </c>
       <c r="T93" t="inlineStr">
         <is>
-          <t>MEDIA THE SQUAD DEMOCRATS ISRAEL</t>
+          <t xml:space="preserve">MEDIA THE SQUAD DEMOCRATS ISRAEL </t>
         </is>
       </c>
     </row>
@@ -7671,7 +7671,7 @@
       </c>
       <c r="T94" t="inlineStr">
         <is>
-          <t xml:space="preserve">CHINA TARIFFS TRADE </t>
+          <t xml:space="preserve">CHINA TARIFFS TRADE  </t>
         </is>
       </c>
     </row>
@@ -7743,7 +7743,7 @@
       </c>
       <c r="T95" t="inlineStr">
         <is>
-          <t xml:space="preserve">MUELLER INVESTIGATION   </t>
+          <t xml:space="preserve">MUELLER INVESTIGATION    </t>
         </is>
       </c>
     </row>
@@ -7818,7 +7818,7 @@
       </c>
       <c r="T96" t="inlineStr">
         <is>
-          <t xml:space="preserve">MUELLER INVESTIGATION JAMES COMEY  </t>
+          <t xml:space="preserve">MUELLER INVESTIGATION JAMES COMEY   </t>
         </is>
       </c>
     </row>
@@ -7894,7 +7894,7 @@
       </c>
       <c r="T97" t="inlineStr">
         <is>
-          <t xml:space="preserve">MUELLER INVESTIGATION OBSTRUCTION OF JUSTICE  </t>
+          <t xml:space="preserve">MUELLER INVESTIGATION OBSTRUCTION OF JUSTICE   </t>
         </is>
       </c>
     </row>
@@ -7969,7 +7969,7 @@
       </c>
       <c r="T98" t="inlineStr">
         <is>
-          <t xml:space="preserve">PUERTO RICO CONGRESS  </t>
+          <t xml:space="preserve">PUERTO RICO CONGRESS   </t>
         </is>
       </c>
     </row>
@@ -8041,7 +8041,7 @@
       </c>
       <c r="T99" t="inlineStr">
         <is>
-          <t xml:space="preserve">MILITARY AFGHANISTAN  </t>
+          <t xml:space="preserve">MILITARY AFGHANISTAN   </t>
         </is>
       </c>
     </row>
@@ -8122,7 +8122,7 @@
       </c>
       <c r="T100" t="inlineStr">
         <is>
-          <t xml:space="preserve">NORTH KOREA VETERANS MILITARY </t>
+          <t xml:space="preserve">NORTH KOREA VETERANS MILITARY  </t>
         </is>
       </c>
     </row>
@@ -8200,7 +8200,7 @@
       </c>
       <c r="T101" t="inlineStr">
         <is>
-          <t xml:space="preserve">PRESCRIPTION DRUGS HEALH CARE  </t>
+          <t xml:space="preserve">PRESCRIPTION DRUGS HEALH CARE   </t>
         </is>
       </c>
     </row>
@@ -8275,7 +8275,7 @@
       </c>
       <c r="T102" t="inlineStr">
         <is>
-          <t xml:space="preserve">ECONOMY UNEMPLOYMENT  </t>
+          <t xml:space="preserve">ECONOMY UNEMPLOYMENT   </t>
         </is>
       </c>
     </row>
@@ -8350,7 +8350,7 @@
       </c>
       <c r="T103" t="inlineStr">
         <is>
-          <t xml:space="preserve">ECONOMY UNEMPLOYMENT  </t>
+          <t xml:space="preserve">ECONOMY UNEMPLOYMENT   </t>
         </is>
       </c>
     </row>
@@ -8429,7 +8429,7 @@
       </c>
       <c r="T104" t="inlineStr">
         <is>
-          <t xml:space="preserve">ECONOMY WOMEN UNEMPLOYMENT </t>
+          <t xml:space="preserve">ECONOMY WOMEN UNEMPLOYMENT  </t>
         </is>
       </c>
     </row>
@@ -8500,7 +8500,7 @@
       </c>
       <c r="T105" t="inlineStr">
         <is>
-          <t xml:space="preserve">IRAN   </t>
+          <t xml:space="preserve">IRAN    </t>
         </is>
       </c>
     </row>
@@ -8569,7 +8569,7 @@
       </c>
       <c r="T106" t="inlineStr">
         <is>
-          <t xml:space="preserve">MUELLER INVESTIGATION   </t>
+          <t xml:space="preserve">MUELLER INVESTIGATION    </t>
         </is>
       </c>
     </row>
@@ -8634,7 +8634,7 @@
       </c>
       <c r="T107" t="inlineStr">
         <is>
-          <t xml:space="preserve">MUELLER INVESTIGATION   </t>
+          <t xml:space="preserve">MUELLER INVESTIGATION    </t>
         </is>
       </c>
     </row>
@@ -8711,7 +8711,7 @@
       </c>
       <c r="T108" t="inlineStr">
         <is>
-          <t xml:space="preserve">IRAN BARACK OBAMA  </t>
+          <t xml:space="preserve">IRAN BARACK OBAMA   </t>
         </is>
       </c>
     </row>
@@ -8792,7 +8792,7 @@
       </c>
       <c r="T109" t="inlineStr">
         <is>
-          <t xml:space="preserve">ECONOMY UNEMPLOYMENT MILITARY </t>
+          <t xml:space="preserve">ECONOMY UNEMPLOYMENT MILITARY  </t>
         </is>
       </c>
     </row>
@@ -8868,7 +8868,7 @@
       </c>
       <c r="T110" t="inlineStr">
         <is>
-          <t xml:space="preserve">PUERTO RICO POPULARITY  </t>
+          <t xml:space="preserve">PUERTO RICO POPULARITY   </t>
         </is>
       </c>
     </row>
@@ -8943,7 +8943,7 @@
       </c>
       <c r="T111" t="inlineStr">
         <is>
-          <t xml:space="preserve">POLLS IMPEACHMENT  </t>
+          <t xml:space="preserve">POLLS IMPEACHMENT   </t>
         </is>
       </c>
     </row>
@@ -9003,7 +9003,7 @@
       </c>
       <c r="T112" t="inlineStr">
         <is>
-          <t xml:space="preserve">POLLS   </t>
+          <t xml:space="preserve">POLLS    </t>
         </is>
       </c>
     </row>
@@ -9078,7 +9078,7 @@
       </c>
       <c r="T113" t="inlineStr">
         <is>
-          <t xml:space="preserve">PAST PRESIDENTS MILITARY  </t>
+          <t xml:space="preserve">PAST PRESIDENTS MILITARY   </t>
         </is>
       </c>
     </row>
@@ -9153,7 +9153,7 @@
       </c>
       <c r="T114" t="inlineStr">
         <is>
-          <t xml:space="preserve">ECONOMY UNEMPLOYMENT  </t>
+          <t xml:space="preserve">ECONOMY UNEMPLOYMENT   </t>
         </is>
       </c>
     </row>
@@ -9230,7 +9230,7 @@
       </c>
       <c r="T115" t="inlineStr">
         <is>
-          <t xml:space="preserve">CHINA TARIFFS TRADE </t>
+          <t xml:space="preserve">CHINA TARIFFS TRADE  </t>
         </is>
       </c>
     </row>
@@ -9301,7 +9301,7 @@
       </c>
       <c r="T116" t="inlineStr">
         <is>
-          <t xml:space="preserve">COURTS   </t>
+          <t xml:space="preserve">COURTS    </t>
         </is>
       </c>
     </row>
@@ -9382,7 +9382,7 @@
       </c>
       <c r="T117" t="inlineStr">
         <is>
-          <t xml:space="preserve">NATO EUROPE MILITARY </t>
+          <t xml:space="preserve">NATO EUROPE MILITARY  </t>
         </is>
       </c>
     </row>
@@ -9463,7 +9463,7 @@
       </c>
       <c r="T118" t="inlineStr">
         <is>
-          <t xml:space="preserve">EUROPE TRADE NATO </t>
+          <t xml:space="preserve">EUROPE TRADE NATO  </t>
         </is>
       </c>
     </row>
@@ -9532,7 +9532,7 @@
       </c>
       <c r="T119" t="inlineStr">
         <is>
-          <t xml:space="preserve">IMMIGRATION CARAVAN  </t>
+          <t xml:space="preserve">IMMIGRATION CARAVAN   </t>
         </is>
       </c>
     </row>
@@ -9601,7 +9601,7 @@
       </c>
       <c r="T120" t="inlineStr">
         <is>
-          <t xml:space="preserve">MEDIA   </t>
+          <t xml:space="preserve">MEDIA    </t>
         </is>
       </c>
     </row>
@@ -9680,7 +9680,7 @@
       </c>
       <c r="T121" t="inlineStr">
         <is>
-          <t>CHINA TARIFFS TRADE FARMERS</t>
+          <t xml:space="preserve">CHINA TARIFFS TRADE FARMERS </t>
         </is>
       </c>
     </row>
@@ -9764,7 +9764,7 @@
       </c>
       <c r="T122" t="inlineStr">
         <is>
-          <t>CHINA TARIFFS PAST PRESIDENTS TRADE</t>
+          <t xml:space="preserve">CHINA TARIFFS PAST PRESIDENTS TRADE </t>
         </is>
       </c>
     </row>
@@ -9848,7 +9848,7 @@
       </c>
       <c r="T123" t="inlineStr">
         <is>
-          <t>CHINA TARIFFS TRADE FARMERS</t>
+          <t xml:space="preserve">CHINA TARIFFS TRADE FARMERS </t>
         </is>
       </c>
     </row>
@@ -9915,7 +9915,7 @@
       </c>
       <c r="T124" t="inlineStr">
         <is>
-          <t xml:space="preserve">MILITARY HEALTH CARE VETERANS </t>
+          <t xml:space="preserve">MILITARY HEALTH CARE VETERANS  </t>
         </is>
       </c>
     </row>
@@ -9992,7 +9992,7 @@
       </c>
       <c r="T125" t="inlineStr">
         <is>
-          <t xml:space="preserve">MILITARY HEALTH CARE VETERANS </t>
+          <t xml:space="preserve">MILITARY HEALTH CARE VETERANS  </t>
         </is>
       </c>
     </row>
@@ -10056,7 +10056,7 @@
       </c>
       <c r="T126" t="inlineStr">
         <is>
-          <t xml:space="preserve">MUELLER INVESTIGATION   </t>
+          <t xml:space="preserve">MUELLER INVESTIGATION    </t>
         </is>
       </c>
     </row>
@@ -10140,7 +10140,7 @@
       </c>
       <c r="T127" t="inlineStr">
         <is>
-          <t xml:space="preserve">VOTER FRAUD CALIFORNIA IMMIGRATION </t>
+          <t xml:space="preserve">VOTER FRAUD CALIFORNIA IMMIGRATION  </t>
         </is>
       </c>
     </row>
@@ -10214,7 +10214,7 @@
       </c>
       <c r="T128" t="inlineStr">
         <is>
-          <t xml:space="preserve">THE SQUAD DEMOCRATS  </t>
+          <t xml:space="preserve">THE SQUAD DEMOCRATS   </t>
         </is>
       </c>
     </row>
@@ -10291,7 +10291,7 @@
       </c>
       <c r="T129" t="inlineStr">
         <is>
-          <t xml:space="preserve">THE SQUAD DEMOCRATS ISRAEL </t>
+          <t xml:space="preserve">THE SQUAD DEMOCRATS ISRAEL  </t>
         </is>
       </c>
     </row>
@@ -10362,7 +10362,7 @@
       </c>
       <c r="T130" t="inlineStr">
         <is>
-          <t xml:space="preserve">SOCIAL MEDIA   </t>
+          <t xml:space="preserve">SOCIAL MEDIA    </t>
         </is>
       </c>
     </row>
@@ -10434,7 +10434,7 @@
       </c>
       <c r="T131" t="inlineStr">
         <is>
-          <t xml:space="preserve">DEMOCRATS IMMIGRATION  </t>
+          <t xml:space="preserve">DEMOCRATS IMMIGRATION   </t>
         </is>
       </c>
     </row>
@@ -10518,7 +10518,7 @@
       </c>
       <c r="T132" t="inlineStr">
         <is>
-          <t>NATO EUROPE TRADE FARMERS</t>
+          <t xml:space="preserve">NATO EUROPE TRADE FARMERS </t>
         </is>
       </c>
     </row>
@@ -10597,7 +10597,7 @@
       </c>
       <c r="T133" t="inlineStr">
         <is>
-          <t xml:space="preserve">NATO MILITARY EUROPE </t>
+          <t xml:space="preserve">NATO MILITARY EUROPE  </t>
         </is>
       </c>
     </row>
@@ -10668,7 +10668,7 @@
       </c>
       <c r="T134" t="inlineStr">
         <is>
-          <t xml:space="preserve">PRESIDENTIAL POWERS   </t>
+          <t xml:space="preserve">PRESIDENTIAL POWERS    </t>
         </is>
       </c>
     </row>
@@ -10748,7 +10748,7 @@
       </c>
       <c r="T135" t="inlineStr">
         <is>
-          <t xml:space="preserve">ENERGY RUSSIA SAUDI ARABIA </t>
+          <t xml:space="preserve">ENERGY RUSSIA SAUDI ARABIA  </t>
         </is>
       </c>
     </row>
@@ -10833,7 +10833,7 @@
       </c>
       <c r="T136" t="inlineStr">
         <is>
-          <t>ENERGY CHINA JAPAN IRAN</t>
+          <t xml:space="preserve">ENERGY CHINA JAPAN IRAN </t>
         </is>
       </c>
     </row>
@@ -10914,7 +10914,7 @@
       </c>
       <c r="T137" t="inlineStr">
         <is>
-          <t xml:space="preserve">DEMOCRATS IMMIGRATION THE WALL </t>
+          <t xml:space="preserve">DEMOCRATS IMMIGRATION THE WALL  </t>
         </is>
       </c>
     </row>
@@ -10989,7 +10989,7 @@
       </c>
       <c r="T138" t="inlineStr">
         <is>
-          <t xml:space="preserve">IMMIGRATION THE WALL  </t>
+          <t xml:space="preserve">IMMIGRATION THE WALL   </t>
         </is>
       </c>
     </row>
@@ -11061,7 +11061,7 @@
       </c>
       <c r="T139" t="inlineStr">
         <is>
-          <t xml:space="preserve">MUELLER INVESTIGATION OBSTRUCTION OF JUSTICE  </t>
+          <t xml:space="preserve">MUELLER INVESTIGATION OBSTRUCTION OF JUSTICE   </t>
         </is>
       </c>
     </row>
@@ -11138,7 +11138,7 @@
       </c>
       <c r="T140" t="inlineStr">
         <is>
-          <t xml:space="preserve">MUELLER INVESTIGATION JAMES COMEY DEMOCRATS </t>
+          <t xml:space="preserve">MUELLER INVESTIGATION JAMES COMEY DEMOCRATS  </t>
         </is>
       </c>
     </row>
@@ -11209,7 +11209,7 @@
       </c>
       <c r="T141" t="inlineStr">
         <is>
-          <t xml:space="preserve">MUELLER INVESTIGATION   </t>
+          <t xml:space="preserve">MUELLER INVESTIGATION    </t>
         </is>
       </c>
     </row>
@@ -11278,7 +11278,7 @@
       </c>
       <c r="T142" t="inlineStr">
         <is>
-          <t xml:space="preserve">MUELLER INVESTIGATION DEMOCRATS  </t>
+          <t xml:space="preserve">MUELLER INVESTIGATION DEMOCRATS   </t>
         </is>
       </c>
     </row>
@@ -11355,7 +11355,7 @@
       </c>
       <c r="T143" t="inlineStr">
         <is>
-          <t xml:space="preserve">HILLARY CLINTON MUELLER INVESTIGATION DEMOCRATS </t>
+          <t xml:space="preserve">HILLARY CLINTON MUELLER INVESTIGATION DEMOCRATS  </t>
         </is>
       </c>
     </row>
@@ -11421,7 +11421,7 @@
       </c>
       <c r="T144" t="inlineStr">
         <is>
-          <t xml:space="preserve">MUELLER INVESTIGATION MEDIA  </t>
+          <t xml:space="preserve">MUELLER INVESTIGATION MEDIA   </t>
         </is>
       </c>
     </row>
@@ -11481,7 +11481,7 @@
       </c>
       <c r="T145" t="inlineStr">
         <is>
-          <t xml:space="preserve">MUELLER INVESTIGATION   </t>
+          <t xml:space="preserve">MUELLER INVESTIGATION    </t>
         </is>
       </c>
     </row>
@@ -11547,7 +11547,7 @@
       </c>
       <c r="T146" t="inlineStr">
         <is>
-          <t xml:space="preserve">ECONOMY UNEMPLOYMENT  </t>
+          <t xml:space="preserve">ECONOMY UNEMPLOYMENT   </t>
         </is>
       </c>
     </row>
@@ -11628,7 +11628,7 @@
       </c>
       <c r="T147" t="inlineStr">
         <is>
-          <t xml:space="preserve">NORTH KOREA MILITARY VETERANS </t>
+          <t xml:space="preserve">NORTH KOREA MILITARY VETERANS  </t>
         </is>
       </c>
     </row>
@@ -11703,7 +11703,7 @@
       </c>
       <c r="T148" t="inlineStr">
         <is>
-          <t xml:space="preserve">RUSSIA MUELLER INVESTIGATION  </t>
+          <t xml:space="preserve">RUSSIA MUELLER INVESTIGATION   </t>
         </is>
       </c>
     </row>
@@ -11772,7 +11772,7 @@
       </c>
       <c r="T149" t="inlineStr">
         <is>
-          <t xml:space="preserve">MUELLER INVESTIGATION   </t>
+          <t xml:space="preserve">MUELLER INVESTIGATION    </t>
         </is>
       </c>
     </row>
@@ -11839,7 +11839,7 @@
       </c>
       <c r="T150" t="inlineStr">
         <is>
-          <t xml:space="preserve">MUELLER INVESTIGATION   </t>
+          <t xml:space="preserve">MUELLER INVESTIGATION    </t>
         </is>
       </c>
     </row>
@@ -11908,7 +11908,7 @@
       </c>
       <c r="T151" t="inlineStr">
         <is>
-          <t xml:space="preserve">MUELLER INVESTIGATION   </t>
+          <t xml:space="preserve">MUELLER INVESTIGATION    </t>
         </is>
       </c>
     </row>
@@ -11983,7 +11983,7 @@
       </c>
       <c r="T152" t="inlineStr">
         <is>
-          <t xml:space="preserve">CROWDS {P[I;AROTY  </t>
+          <t xml:space="preserve">CROWDS {P[I;AROTY   </t>
         </is>
       </c>
     </row>
@@ -12063,7 +12063,7 @@
       </c>
       <c r="T153" t="inlineStr">
         <is>
-          <t xml:space="preserve">ENERGY RUSSIA SAUDI ARABIA </t>
+          <t xml:space="preserve">ENERGY RUSSIA SAUDI ARABIA  </t>
         </is>
       </c>
     </row>
@@ -12139,7 +12139,7 @@
       </c>
       <c r="T154" t="inlineStr">
         <is>
-          <t xml:space="preserve">NORTH KOREA MILITARY  </t>
+          <t xml:space="preserve">NORTH KOREA MILITARY   </t>
         </is>
       </c>
     </row>
@@ -12213,7 +12213,7 @@
       </c>
       <c r="T155" t="inlineStr">
         <is>
-          <t xml:space="preserve">MUELLER INVESTIGATION COLLUSION  </t>
+          <t xml:space="preserve">MUELLER INVESTIGATION COLLUSION   </t>
         </is>
       </c>
     </row>
@@ -12282,7 +12282,7 @@
       </c>
       <c r="T156" t="inlineStr">
         <is>
-          <t xml:space="preserve">MUELLER INVESTIGATION   </t>
+          <t xml:space="preserve">MUELLER INVESTIGATION    </t>
         </is>
       </c>
     </row>
@@ -12354,7 +12354,7 @@
       </c>
       <c r="T157" t="inlineStr">
         <is>
-          <t xml:space="preserve">TURKEY MILITARY  </t>
+          <t xml:space="preserve">TURKEY MILITARY   </t>
         </is>
       </c>
     </row>
@@ -12430,7 +12430,7 @@
       </c>
       <c r="T158" t="inlineStr">
         <is>
-          <t xml:space="preserve">ECONOMY UNEMPLOYMENT  </t>
+          <t xml:space="preserve">ECONOMY UNEMPLOYMENT   </t>
         </is>
       </c>
     </row>
@@ -12510,7 +12510,7 @@
       </c>
       <c r="T159" t="inlineStr">
         <is>
-          <t xml:space="preserve">CHINA TARIFFS TRADE </t>
+          <t xml:space="preserve">CHINA TARIFFS TRADE  </t>
         </is>
       </c>
     </row>
@@ -12584,7 +12584,7 @@
       </c>
       <c r="T160" t="inlineStr">
         <is>
-          <t xml:space="preserve">CHINA TRADE  </t>
+          <t xml:space="preserve">CHINA TRADE   </t>
         </is>
       </c>
     </row>
@@ -12663,7 +12663,7 @@
       </c>
       <c r="T161" t="inlineStr">
         <is>
-          <t xml:space="preserve">CHINA TRADE TARIFFS </t>
+          <t xml:space="preserve">CHINA TRADE TARIFFS  </t>
         </is>
       </c>
     </row>
@@ -12748,7 +12748,7 @@
       </c>
       <c r="T162" t="inlineStr">
         <is>
-          <t>CHINA TARIFFS TRADE FARMERS</t>
+          <t xml:space="preserve">CHINA TARIFFS TRADE FARMERS </t>
         </is>
       </c>
     </row>
@@ -12823,7 +12823,7 @@
       </c>
       <c r="T163" t="inlineStr">
         <is>
-          <t xml:space="preserve">CHINA TRADE  </t>
+          <t xml:space="preserve">CHINA TRADE   </t>
         </is>
       </c>
     </row>
@@ -12897,7 +12897,7 @@
       </c>
       <c r="T164" t="inlineStr">
         <is>
-          <t xml:space="preserve">DEMOCRATS IMMIGRATION  </t>
+          <t xml:space="preserve">DEMOCRATS IMMIGRATION   </t>
         </is>
       </c>
     </row>
@@ -12978,7 +12978,7 @@
       </c>
       <c r="T165" t="inlineStr">
         <is>
-          <t xml:space="preserve">DEMOCRATS IMMIGRATION THE WALL </t>
+          <t xml:space="preserve">DEMOCRATS IMMIGRATION THE WALL  </t>
         </is>
       </c>
     </row>
@@ -13053,7 +13053,7 @@
       </c>
       <c r="T166" t="inlineStr">
         <is>
-          <t xml:space="preserve">MEXICO IMMIGRATION  </t>
+          <t xml:space="preserve">MEXICO IMMIGRATION   </t>
         </is>
       </c>
     </row>
@@ -13128,7 +13128,7 @@
       </c>
       <c r="T167" t="inlineStr">
         <is>
-          <t xml:space="preserve">IMMIGRATION THE WALL  </t>
+          <t xml:space="preserve">IMMIGRATION THE WALL   </t>
         </is>
       </c>
     </row>
@@ -13202,7 +13202,7 @@
       </c>
       <c r="T168" t="inlineStr">
         <is>
-          <t xml:space="preserve">CONGRESS DEMOCRATS  </t>
+          <t xml:space="preserve">CONGRESS DEMOCRATS   </t>
         </is>
       </c>
     </row>
@@ -13267,7 +13267,7 @@
       </c>
       <c r="T169" t="inlineStr">
         <is>
-          <t xml:space="preserve">MUELLER INVESTIGATION   </t>
+          <t xml:space="preserve">MUELLER INVESTIGATION    </t>
         </is>
       </c>
     </row>
@@ -13346,7 +13346,7 @@
       </c>
       <c r="T170" t="inlineStr">
         <is>
-          <t>MUELLER INVESTIGATION HILLARY CLINTON DEMOCRATS COLLUSION</t>
+          <t xml:space="preserve">MUELLER INVESTIGATION HILLARY CLINTON DEMOCRATS COLLUSION </t>
         </is>
       </c>
     </row>
@@ -13415,7 +13415,7 @@
       </c>
       <c r="T171" t="inlineStr">
         <is>
-          <t xml:space="preserve">DEMOCRATS IMMIGRATION  </t>
+          <t xml:space="preserve">DEMOCRATS IMMIGRATION   </t>
         </is>
       </c>
     </row>
@@ -13484,7 +13484,7 @@
       </c>
       <c r="T172" t="inlineStr">
         <is>
-          <t xml:space="preserve">BALTIMORE DEMOCRATS  </t>
+          <t xml:space="preserve">BALTIMORE DEMOCRATS   </t>
         </is>
       </c>
     </row>
@@ -13560,7 +13560,7 @@
       </c>
       <c r="T173" t="inlineStr">
         <is>
-          <t xml:space="preserve">EUROPE ECONOMY TRADE </t>
+          <t xml:space="preserve">EUROPE ECONOMY TRADE  </t>
         </is>
       </c>
     </row>
@@ -13636,7 +13636,7 @@
       </c>
       <c r="T174" t="inlineStr">
         <is>
-          <t xml:space="preserve">THE WALL IMMIGRATION DEMOCRATS </t>
+          <t xml:space="preserve">THE WALL IMMIGRATION DEMOCRATS  </t>
         </is>
       </c>
     </row>
@@ -13706,7 +13706,7 @@
       </c>
       <c r="T175" t="inlineStr">
         <is>
-          <t xml:space="preserve">CROWDS POPULARITY  </t>
+          <t xml:space="preserve">CROWDS POPULARITY   </t>
         </is>
       </c>
     </row>
@@ -13771,7 +13771,7 @@
       </c>
       <c r="T176" t="inlineStr">
         <is>
-          <t xml:space="preserve">MEDIA   </t>
+          <t xml:space="preserve">MEDIA    </t>
         </is>
       </c>
     </row>
@@ -13847,7 +13847,7 @@
       </c>
       <c r="T177" t="inlineStr">
         <is>
-          <t xml:space="preserve">CROWDS 2020 DEMOCRATIC CANDIDATES JOE BIDEN </t>
+          <t xml:space="preserve">CROWDS 2020 DEMOCRATIC CANDIDATES JOE BIDEN  </t>
         </is>
       </c>
     </row>
@@ -13915,7 +13915,7 @@
       </c>
       <c r="T178" t="inlineStr">
         <is>
-          <t xml:space="preserve">DEMOCRATS IMMIGRATION  </t>
+          <t xml:space="preserve">DEMOCRATS IMMIGRATION   </t>
         </is>
       </c>
     </row>
@@ -13989,7 +13989,7 @@
       </c>
       <c r="T179" t="inlineStr">
         <is>
-          <t xml:space="preserve">MILITARY VETERANS HEALTH CARE </t>
+          <t xml:space="preserve">MILITARY VETERANS HEALTH CARE  </t>
         </is>
       </c>
     </row>
@@ -14064,7 +14064,7 @@
       </c>
       <c r="T180" t="inlineStr">
         <is>
-          <t>CHINA TARIFFS TRADE FARMERS</t>
+          <t xml:space="preserve">CHINA TARIFFS TRADE FARMERS </t>
         </is>
       </c>
     </row>
@@ -14142,7 +14142,7 @@
       </c>
       <c r="T181" t="inlineStr">
         <is>
-          <t>CHINA TARIFFS TRADE ECONOMY</t>
+          <t xml:space="preserve">CHINA TARIFFS TRADE ECONOMY </t>
         </is>
       </c>
     </row>
@@ -14212,7 +14212,7 @@
       </c>
       <c r="T182" t="inlineStr">
         <is>
-          <t xml:space="preserve">MUELLER INVESTIGATION COURTS  </t>
+          <t xml:space="preserve">MUELLER INVESTIGATION COURTS   </t>
         </is>
       </c>
     </row>
@@ -14275,7 +14275,7 @@
       </c>
       <c r="T183" t="inlineStr">
         <is>
-          <t xml:space="preserve">DEMOCRATS IMMIGRATION  </t>
+          <t xml:space="preserve">DEMOCRATS IMMIGRATION   </t>
         </is>
       </c>
     </row>
@@ -14347,7 +14347,7 @@
       </c>
       <c r="T184" t="inlineStr">
         <is>
-          <t xml:space="preserve">IMMIGRATION BARACK OBAMA  </t>
+          <t xml:space="preserve">IMMIGRATION BARACK OBAMA   </t>
         </is>
       </c>
     </row>
@@ -14415,7 +14415,7 @@
       </c>
       <c r="T185" t="inlineStr">
         <is>
-          <t xml:space="preserve">IMMIGRATION   </t>
+          <t xml:space="preserve">IMMIGRATION    </t>
         </is>
       </c>
     </row>
@@ -14486,7 +14486,7 @@
       </c>
       <c r="T186" t="inlineStr">
         <is>
-          <t xml:space="preserve">COURTS   </t>
+          <t xml:space="preserve">COURTS    </t>
         </is>
       </c>
     </row>
@@ -14550,7 +14550,7 @@
       </c>
       <c r="T187" t="inlineStr">
         <is>
-          <t xml:space="preserve">POLLS POPULARITY  </t>
+          <t xml:space="preserve">POLLS POPULARITY   </t>
         </is>
       </c>
     </row>
@@ -14615,7 +14615,7 @@
       </c>
       <c r="T188" t="inlineStr">
         <is>
-          <t xml:space="preserve">CROWDS POPULARITY  </t>
+          <t xml:space="preserve">CROWDS POPULARITY   </t>
         </is>
       </c>
     </row>
@@ -14687,7 +14687,7 @@
       </c>
       <c r="T189" t="inlineStr">
         <is>
-          <t xml:space="preserve">ROBERT MUELLER OBSTRUCTION OF JUSTICE COLLUSION </t>
+          <t xml:space="preserve">ROBERT MUELLER OBSTRUCTION OF JUSTICE COLLUSION  </t>
         </is>
       </c>
     </row>
@@ -14760,7 +14760,7 @@
       </c>
       <c r="T190" t="inlineStr">
         <is>
-          <t xml:space="preserve">DEMOCRATS IMMIGRATION  </t>
+          <t xml:space="preserve">DEMOCRATS IMMIGRATION   </t>
         </is>
       </c>
     </row>
@@ -14828,7 +14828,7 @@
       </c>
       <c r="T191" t="inlineStr">
         <is>
-          <t xml:space="preserve">DEMOCRATS IMMIGRATION  </t>
+          <t xml:space="preserve">DEMOCRATS IMMIGRATION   </t>
         </is>
       </c>
     </row>
@@ -14903,7 +14903,7 @@
       </c>
       <c r="T192" t="inlineStr">
         <is>
-          <t xml:space="preserve">CROWDS POPULARITY  </t>
+          <t xml:space="preserve">CROWDS POPULARITY   </t>
         </is>
       </c>
     </row>
@@ -14985,7 +14985,7 @@
       </c>
       <c r="T193" t="inlineStr">
         <is>
-          <t xml:space="preserve">TARIFFS STEEL ECONOMY </t>
+          <t xml:space="preserve">TARIFFS STEEL ECONOMY  </t>
         </is>
       </c>
     </row>
@@ -15067,7 +15067,7 @@
       </c>
       <c r="T194" t="inlineStr">
         <is>
-          <t xml:space="preserve">TARIFFS STEEL ECONOMY </t>
+          <t xml:space="preserve">TARIFFS STEEL ECONOMY  </t>
         </is>
       </c>
     </row>
@@ -15141,7 +15141,7 @@
       </c>
       <c r="T195" t="inlineStr">
         <is>
-          <t xml:space="preserve">2016 ELECTION OHIO  </t>
+          <t xml:space="preserve">2016 ELECTION OHIO   </t>
         </is>
       </c>
     </row>
@@ -15215,7 +15215,7 @@
       </c>
       <c r="T196" t="inlineStr">
         <is>
-          <t xml:space="preserve">2016 ELECTION POPULARITY  </t>
+          <t xml:space="preserve">2016 ELECTION POPULARITY   </t>
         </is>
       </c>
     </row>
@@ -15289,7 +15289,7 @@
       </c>
       <c r="T197" t="inlineStr">
         <is>
-          <t xml:space="preserve">2016 ELECTION FLORIDA  </t>
+          <t xml:space="preserve">2016 ELECTION FLORIDA   </t>
         </is>
       </c>
     </row>
@@ -15368,7 +15368,7 @@
       </c>
       <c r="T198" t="inlineStr">
         <is>
-          <t xml:space="preserve">VETERANS HEALTH CARE MILITARY </t>
+          <t xml:space="preserve">VETERANS HEALTH CARE MILITARY  </t>
         </is>
       </c>
     </row>
@@ -15450,7 +15450,7 @@
       </c>
       <c r="T199" t="inlineStr">
         <is>
-          <t xml:space="preserve">VETERANS HEALTH CARE MILITARY </t>
+          <t xml:space="preserve">VETERANS HEALTH CARE MILITARY  </t>
         </is>
       </c>
     </row>
@@ -15524,7 +15524,7 @@
       </c>
       <c r="T200" t="inlineStr">
         <is>
-          <t xml:space="preserve">RIGHT TO TRY HEALTH CARE  </t>
+          <t xml:space="preserve">RIGHT TO TRY HEALTH CARE   </t>
         </is>
       </c>
     </row>
@@ -15599,7 +15599,7 @@
       </c>
       <c r="T201" t="inlineStr">
         <is>
-          <t xml:space="preserve">RIGHT TO TRY HEALTH CARE  </t>
+          <t xml:space="preserve">RIGHT TO TRY HEALTH CARE   </t>
         </is>
       </c>
     </row>
@@ -15668,7 +15668,7 @@
       </c>
       <c r="T202" t="inlineStr">
         <is>
-          <t xml:space="preserve">HEALTH CARE   </t>
+          <t xml:space="preserve">HEALTH CARE    </t>
         </is>
       </c>
     </row>
@@ -15742,7 +15742,7 @@
       </c>
       <c r="T203" t="inlineStr">
         <is>
-          <t xml:space="preserve">IMMIGRATION DEMOCRATS  </t>
+          <t xml:space="preserve">IMMIGRATION DEMOCRATS   </t>
         </is>
       </c>
     </row>
@@ -15816,7 +15816,7 @@
       </c>
       <c r="T204" t="inlineStr">
         <is>
-          <t xml:space="preserve">ENERGY BARACK OBAMA  </t>
+          <t xml:space="preserve">ENERGY BARACK OBAMA   </t>
         </is>
       </c>
     </row>
@@ -15885,7 +15885,7 @@
       </c>
       <c r="T205" t="inlineStr">
         <is>
-          <t xml:space="preserve">BARACK OBAMA ECONOMY  </t>
+          <t xml:space="preserve">BARACK OBAMA ECONOMY   </t>
         </is>
       </c>
     </row>
@@ -15959,7 +15959,7 @@
       </c>
       <c r="T206" t="inlineStr">
         <is>
-          <t xml:space="preserve">BARACK OBAMA ECONOMY  </t>
+          <t xml:space="preserve">BARACK OBAMA ECONOMY   </t>
         </is>
       </c>
     </row>
@@ -16033,7 +16033,7 @@
       </c>
       <c r="T207" t="inlineStr">
         <is>
-          <t xml:space="preserve">ENERGY BARACK OBAMA  </t>
+          <t xml:space="preserve">ENERGY BARACK OBAMA   </t>
         </is>
       </c>
     </row>
@@ -16109,7 +16109,7 @@
       </c>
       <c r="T208" t="inlineStr">
         <is>
-          <t xml:space="preserve">ENERGY BARACK OBAMA  </t>
+          <t xml:space="preserve">ENERGY BARACK OBAMA   </t>
         </is>
       </c>
     </row>
@@ -16187,7 +16187,7 @@
       </c>
       <c r="T209" t="inlineStr">
         <is>
-          <t xml:space="preserve">BARACK OBAMA IRAN  </t>
+          <t xml:space="preserve">BARACK OBAMA IRAN   </t>
         </is>
       </c>
     </row>
@@ -16263,7 +16263,7 @@
       </c>
       <c r="T210" t="inlineStr">
         <is>
-          <t xml:space="preserve">THE WALL IMMIGRATION  </t>
+          <t xml:space="preserve">THE WALL IMMIGRATION   </t>
         </is>
       </c>
     </row>
@@ -16337,7 +16337,7 @@
       </c>
       <c r="T211" t="inlineStr">
         <is>
-          <t xml:space="preserve">IMMIGRATION DEMOCRATS  </t>
+          <t xml:space="preserve">IMMIGRATION DEMOCRATS   </t>
         </is>
       </c>
     </row>
@@ -16416,7 +16416,7 @@
       </c>
       <c r="T212" t="inlineStr">
         <is>
-          <t xml:space="preserve">ECONOMY JOBS UNEMPLOYMENT </t>
+          <t xml:space="preserve">ECONOMY JOBS UNEMPLOYMENT  </t>
         </is>
       </c>
     </row>
@@ -16495,7 +16495,7 @@
       </c>
       <c r="T213" t="inlineStr">
         <is>
-          <t xml:space="preserve">ECONOMY JOBS UNEMPLOYMENT </t>
+          <t xml:space="preserve">ECONOMY JOBS UNEMPLOYMENT  </t>
         </is>
       </c>
     </row>
@@ -16572,7 +16572,7 @@
       </c>
       <c r="T214" t="inlineStr">
         <is>
-          <t xml:space="preserve">ECONOMY JOBS UNEMPLOYMENT </t>
+          <t xml:space="preserve">ECONOMY JOBS UNEMPLOYMENT  </t>
         </is>
       </c>
     </row>
@@ -16641,7 +16641,7 @@
       </c>
       <c r="T215" t="inlineStr">
         <is>
-          <t xml:space="preserve">COURTS   </t>
+          <t xml:space="preserve">COURTS    </t>
         </is>
       </c>
     </row>
@@ -16721,7 +16721,7 @@
       </c>
       <c r="T216" t="inlineStr">
         <is>
-          <t xml:space="preserve">HEALTH CARE PRESCRIPTION DRUGS HEALTH CARE </t>
+          <t xml:space="preserve">HEALTH CARE PRESCRIPTION DRUGS HEALTH CARE  </t>
         </is>
       </c>
     </row>
@@ -16799,7 +16799,7 @@
       </c>
       <c r="T217" t="inlineStr">
         <is>
-          <t>CHINA TARIFFS TRADE ECONOMY</t>
+          <t xml:space="preserve">CHINA TARIFFS TRADE ECONOMY </t>
         </is>
       </c>
     </row>
@@ -16887,7 +16887,7 @@
       </c>
       <c r="T218" t="inlineStr">
         <is>
-          <t>CHINA TARIFFS TRADE ECONOMY</t>
+          <t xml:space="preserve">CHINA TARIFFS TRADE ECONOMY </t>
         </is>
       </c>
     </row>
@@ -16944,7 +16944,7 @@
       </c>
       <c r="T219" t="inlineStr">
         <is>
-          <t xml:space="preserve">AFGHANISTAN   </t>
+          <t xml:space="preserve">AFGHANISTAN    </t>
         </is>
       </c>
     </row>
@@ -17015,7 +17015,7 @@
       </c>
       <c r="T220" t="inlineStr">
         <is>
-          <t xml:space="preserve">RUSSIA CHINA MILITARY </t>
+          <t xml:space="preserve">RUSSIA CHINA MILITARY  </t>
         </is>
       </c>
     </row>
@@ -17093,7 +17093,7 @@
       </c>
       <c r="T221" t="inlineStr">
         <is>
-          <t>CHINA TARIFFS TRADE ECONOMY</t>
+          <t xml:space="preserve">CHINA TARIFFS TRADE ECONOMY </t>
         </is>
       </c>
     </row>
@@ -17167,7 +17167,7 @@
       </c>
       <c r="T222" t="inlineStr">
         <is>
-          <t>CHINA TARIFFS TRADE ECONOMY</t>
+          <t xml:space="preserve">CHINA TARIFFS TRADE ECONOMY </t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added start of isoweek date field, substituted it for time-based tab
</commit_message>
<xml_diff>
--- a/saved_versions/fcheck_temp.xlsx
+++ b/saved_versions/fcheck_temp.xlsx
@@ -355,13 +355,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P380"/>
+  <dimension ref="A1:Q380"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" style="2" customWidth="1"/>
+    <col min="17" max="17" width="20.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1">
@@ -445,6 +446,11 @@
           <t>isoweek</t>
         </is>
       </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>isoweek_floor_date</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2">
@@ -503,6 +509,9 @@
       <c r="P2">
         <v>28</v>
       </c>
+      <c r="Q2" s="2">
+        <v>43654</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2">
@@ -561,6 +570,9 @@
       <c r="P3">
         <v>28</v>
       </c>
+      <c r="Q3" s="2">
+        <v>43654</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2">
@@ -620,6 +632,9 @@
       <c r="P4">
         <v>28</v>
       </c>
+      <c r="Q4" s="2">
+        <v>43654</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2">
@@ -684,6 +699,9 @@
       <c r="P5">
         <v>28</v>
       </c>
+      <c r="Q5" s="2">
+        <v>43654</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2">
@@ -747,6 +765,9 @@
       <c r="P6">
         <v>28</v>
       </c>
+      <c r="Q6" s="2">
+        <v>43654</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2">
@@ -805,6 +826,9 @@
       <c r="P7">
         <v>28</v>
       </c>
+      <c r="Q7" s="2">
+        <v>43654</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2">
@@ -863,6 +887,9 @@
       <c r="P8">
         <v>28</v>
       </c>
+      <c r="Q8" s="2">
+        <v>43654</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2">
@@ -921,6 +948,9 @@
       <c r="P9">
         <v>28</v>
       </c>
+      <c r="Q9" s="2">
+        <v>43654</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2">
@@ -980,6 +1010,9 @@
       <c r="P10">
         <v>28</v>
       </c>
+      <c r="Q10" s="2">
+        <v>43654</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2">
@@ -1038,6 +1071,9 @@
       <c r="P11">
         <v>28</v>
       </c>
+      <c r="Q11" s="2">
+        <v>43654</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="2">
@@ -1096,6 +1132,9 @@
       <c r="P12">
         <v>28</v>
       </c>
+      <c r="Q12" s="2">
+        <v>43654</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="2">
@@ -1154,6 +1193,9 @@
       <c r="P13">
         <v>28</v>
       </c>
+      <c r="Q13" s="2">
+        <v>43654</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="2">
@@ -1212,6 +1254,9 @@
       </c>
       <c r="P14">
         <v>28</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>43654</v>
       </c>
     </row>
     <row r="15">
@@ -1275,6 +1320,9 @@
       <c r="P15">
         <v>28</v>
       </c>
+      <c r="Q15" s="2">
+        <v>43654</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2">
@@ -1332,6 +1380,9 @@
       </c>
       <c r="P16">
         <v>28</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>43654</v>
       </c>
     </row>
     <row r="17">
@@ -1393,6 +1444,9 @@
       <c r="P17">
         <v>28</v>
       </c>
+      <c r="Q17" s="2">
+        <v>43654</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="2">
@@ -1453,6 +1507,9 @@
       <c r="P18">
         <v>28</v>
       </c>
+      <c r="Q18" s="2">
+        <v>43654</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="2">
@@ -1511,6 +1568,9 @@
       <c r="P19">
         <v>28</v>
       </c>
+      <c r="Q19" s="2">
+        <v>43654</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="2">
@@ -1570,6 +1630,9 @@
       <c r="P20">
         <v>28</v>
       </c>
+      <c r="Q20" s="2">
+        <v>43654</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="2">
@@ -1639,6 +1702,9 @@
       <c r="P21">
         <v>28</v>
       </c>
+      <c r="Q21" s="2">
+        <v>43654</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="2">
@@ -1703,6 +1769,9 @@
       <c r="P22">
         <v>28</v>
       </c>
+      <c r="Q22" s="2">
+        <v>43654</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="2">
@@ -1766,6 +1835,9 @@
       <c r="P23">
         <v>28</v>
       </c>
+      <c r="Q23" s="2">
+        <v>43654</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="2">
@@ -1830,6 +1902,9 @@
       <c r="P24">
         <v>28</v>
       </c>
+      <c r="Q24" s="2">
+        <v>43654</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="2">
@@ -1894,6 +1969,9 @@
       <c r="P25">
         <v>28</v>
       </c>
+      <c r="Q25" s="2">
+        <v>43654</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="2">
@@ -1957,6 +2035,9 @@
       <c r="P26">
         <v>28</v>
       </c>
+      <c r="Q26" s="2">
+        <v>43654</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="2">
@@ -2019,6 +2100,9 @@
       </c>
       <c r="P27">
         <v>28</v>
+      </c>
+      <c r="Q27" s="2">
+        <v>43654</v>
       </c>
     </row>
     <row r="28">
@@ -2087,6 +2171,9 @@
       <c r="P28">
         <v>28</v>
       </c>
+      <c r="Q28" s="2">
+        <v>43654</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="2">
@@ -2150,6 +2237,9 @@
       <c r="P29">
         <v>28</v>
       </c>
+      <c r="Q29" s="2">
+        <v>43654</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="2">
@@ -2213,6 +2303,9 @@
       <c r="P30">
         <v>28</v>
       </c>
+      <c r="Q30" s="2">
+        <v>43654</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="2">
@@ -2266,6 +2359,9 @@
       <c r="P31">
         <v>28</v>
       </c>
+      <c r="Q31" s="2">
+        <v>43654</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="2">
@@ -2323,6 +2419,9 @@
       </c>
       <c r="P32">
         <v>29</v>
+      </c>
+      <c r="Q32" s="2">
+        <v>43661</v>
       </c>
     </row>
     <row r="33">
@@ -2388,6 +2487,9 @@
       <c r="P33">
         <v>29</v>
       </c>
+      <c r="Q33" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="2">
@@ -2442,6 +2544,9 @@
       <c r="P34">
         <v>29</v>
       </c>
+      <c r="Q34" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="2">
@@ -2496,6 +2601,9 @@
       <c r="P35">
         <v>29</v>
       </c>
+      <c r="Q35" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="2">
@@ -2550,6 +2658,9 @@
       <c r="P36">
         <v>29</v>
       </c>
+      <c r="Q36" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="2">
@@ -2602,6 +2713,9 @@
       <c r="P37">
         <v>29</v>
       </c>
+      <c r="Q37" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="2">
@@ -2666,6 +2780,9 @@
       <c r="P38">
         <v>29</v>
       </c>
+      <c r="Q38" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="2">
@@ -2728,6 +2845,9 @@
       </c>
       <c r="P39">
         <v>29</v>
+      </c>
+      <c r="Q39" s="2">
+        <v>43661</v>
       </c>
     </row>
     <row r="40">
@@ -2794,6 +2914,9 @@
       <c r="P40">
         <v>29</v>
       </c>
+      <c r="Q40" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="2">
@@ -2857,6 +2980,9 @@
       <c r="P41">
         <v>29</v>
       </c>
+      <c r="Q41" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="2">
@@ -2921,6 +3047,9 @@
       <c r="P42">
         <v>29</v>
       </c>
+      <c r="Q42" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="2">
@@ -2985,6 +3114,9 @@
       <c r="P43">
         <v>29</v>
       </c>
+      <c r="Q43" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="2">
@@ -3048,6 +3180,9 @@
       <c r="P44">
         <v>29</v>
       </c>
+      <c r="Q44" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="2">
@@ -3112,6 +3247,9 @@
       <c r="P45">
         <v>29</v>
       </c>
+      <c r="Q45" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="2">
@@ -3175,6 +3313,9 @@
       <c r="P46">
         <v>29</v>
       </c>
+      <c r="Q46" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="2">
@@ -3238,6 +3379,9 @@
       <c r="P47">
         <v>29</v>
       </c>
+      <c r="Q47" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="2">
@@ -3301,6 +3445,9 @@
       <c r="P48">
         <v>29</v>
       </c>
+      <c r="Q48" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="2">
@@ -3363,6 +3510,9 @@
       </c>
       <c r="P49">
         <v>29</v>
+      </c>
+      <c r="Q49" s="2">
+        <v>43661</v>
       </c>
     </row>
     <row r="50">
@@ -3430,6 +3580,9 @@
       <c r="P50">
         <v>29</v>
       </c>
+      <c r="Q50" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="2">
@@ -3490,6 +3643,9 @@
       <c r="P51">
         <v>29</v>
       </c>
+      <c r="Q51" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="2">
@@ -3555,6 +3711,9 @@
       <c r="P52">
         <v>29</v>
       </c>
+      <c r="Q52" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="2">
@@ -3619,6 +3778,9 @@
       <c r="P53">
         <v>29</v>
       </c>
+      <c r="Q53" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="2">
@@ -3681,6 +3843,9 @@
       <c r="P54">
         <v>29</v>
       </c>
+      <c r="Q54" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="2">
@@ -3749,6 +3914,9 @@
       <c r="P55">
         <v>29</v>
       </c>
+      <c r="Q55" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="2">
@@ -3817,6 +3985,9 @@
       <c r="P56">
         <v>29</v>
       </c>
+      <c r="Q56" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="2">
@@ -3884,6 +4055,9 @@
       <c r="P57">
         <v>29</v>
       </c>
+      <c r="Q57" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="2">
@@ -3953,6 +4127,9 @@
       <c r="P58">
         <v>29</v>
       </c>
+      <c r="Q58" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="2">
@@ -4021,6 +4198,9 @@
       </c>
       <c r="P59">
         <v>29</v>
+      </c>
+      <c r="Q59" s="2">
+        <v>43661</v>
       </c>
     </row>
     <row r="60">
@@ -4092,6 +4272,9 @@
       <c r="P60">
         <v>29</v>
       </c>
+      <c r="Q60" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="2">
@@ -4162,6 +4345,9 @@
       <c r="P61">
         <v>29</v>
       </c>
+      <c r="Q61" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="2">
@@ -4232,6 +4418,9 @@
       <c r="P62">
         <v>29</v>
       </c>
+      <c r="Q62" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="2">
@@ -4301,6 +4490,9 @@
       <c r="P63">
         <v>29</v>
       </c>
+      <c r="Q63" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="2">
@@ -4370,6 +4562,9 @@
       <c r="P64">
         <v>29</v>
       </c>
+      <c r="Q64" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="2">
@@ -4439,6 +4634,9 @@
       <c r="P65">
         <v>29</v>
       </c>
+      <c r="Q65" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="2">
@@ -4506,6 +4704,9 @@
       </c>
       <c r="P66">
         <v>29</v>
+      </c>
+      <c r="Q66" s="2">
+        <v>43661</v>
       </c>
     </row>
     <row r="67">
@@ -4577,6 +4778,9 @@
       <c r="P67">
         <v>29</v>
       </c>
+      <c r="Q67" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="2">
@@ -4646,6 +4850,9 @@
       <c r="P68">
         <v>29</v>
       </c>
+      <c r="Q68" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="2">
@@ -4714,6 +4921,9 @@
       <c r="P69">
         <v>29</v>
       </c>
+      <c r="Q69" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="2">
@@ -4782,6 +4992,9 @@
       <c r="P70">
         <v>29</v>
       </c>
+      <c r="Q70" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="2">
@@ -4849,6 +5062,9 @@
       </c>
       <c r="P71">
         <v>29</v>
+      </c>
+      <c r="Q71" s="2">
+        <v>43661</v>
       </c>
     </row>
     <row r="72">
@@ -4920,6 +5136,9 @@
       <c r="P72">
         <v>29</v>
       </c>
+      <c r="Q72" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="2">
@@ -4988,6 +5207,9 @@
       <c r="P73">
         <v>29</v>
       </c>
+      <c r="Q73" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="2">
@@ -5051,6 +5273,9 @@
       <c r="P74">
         <v>29</v>
       </c>
+      <c r="Q74" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="2">
@@ -5109,6 +5334,9 @@
       </c>
       <c r="P75">
         <v>29</v>
+      </c>
+      <c r="Q75" s="2">
+        <v>43661</v>
       </c>
     </row>
     <row r="76">
@@ -5175,6 +5403,9 @@
       </c>
       <c r="P76">
         <v>29</v>
+      </c>
+      <c r="Q76" s="2">
+        <v>43661</v>
       </c>
     </row>
     <row r="77">
@@ -5241,6 +5472,9 @@
       <c r="P77">
         <v>29</v>
       </c>
+      <c r="Q77" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="2">
@@ -5303,6 +5537,9 @@
       <c r="P78">
         <v>29</v>
       </c>
+      <c r="Q78" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="2">
@@ -5363,6 +5600,9 @@
       <c r="P79">
         <v>29</v>
       </c>
+      <c r="Q79" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="2">
@@ -5421,6 +5661,9 @@
       </c>
       <c r="P80">
         <v>29</v>
+      </c>
+      <c r="Q80" s="2">
+        <v>43661</v>
       </c>
     </row>
     <row r="81">
@@ -5482,6 +5725,9 @@
       <c r="P81">
         <v>29</v>
       </c>
+      <c r="Q81" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="2">
@@ -5540,6 +5786,9 @@
       </c>
       <c r="P82">
         <v>29</v>
+      </c>
+      <c r="Q82" s="2">
+        <v>43661</v>
       </c>
     </row>
     <row r="83">
@@ -5605,6 +5854,9 @@
       <c r="P83">
         <v>29</v>
       </c>
+      <c r="Q83" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="2">
@@ -5664,6 +5916,9 @@
       <c r="P84">
         <v>29</v>
       </c>
+      <c r="Q84" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="2">
@@ -5722,6 +5977,9 @@
       </c>
       <c r="P85">
         <v>29</v>
+      </c>
+      <c r="Q85" s="2">
+        <v>43661</v>
       </c>
     </row>
     <row r="86">
@@ -5782,6 +6040,9 @@
       </c>
       <c r="P86">
         <v>29</v>
+      </c>
+      <c r="Q86" s="2">
+        <v>43661</v>
       </c>
     </row>
     <row r="87">
@@ -5849,6 +6110,9 @@
       <c r="P87">
         <v>29</v>
       </c>
+      <c r="Q87" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="2">
@@ -5902,6 +6166,9 @@
       </c>
       <c r="P88">
         <v>29</v>
+      </c>
+      <c r="Q88" s="2">
+        <v>43661</v>
       </c>
     </row>
     <row r="89">
@@ -5958,6 +6225,9 @@
       </c>
       <c r="P89">
         <v>29</v>
+      </c>
+      <c r="Q89" s="2">
+        <v>43661</v>
       </c>
     </row>
     <row r="90">
@@ -6016,6 +6286,9 @@
       <c r="P90">
         <v>29</v>
       </c>
+      <c r="Q90" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="2">
@@ -6071,6 +6344,9 @@
       <c r="P91">
         <v>29</v>
       </c>
+      <c r="Q91" s="2">
+        <v>43661</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="2">
@@ -6129,6 +6405,9 @@
       </c>
       <c r="P92">
         <v>30</v>
+      </c>
+      <c r="Q92" s="2">
+        <v>43668</v>
       </c>
     </row>
     <row r="93">
@@ -6192,6 +6471,9 @@
       <c r="P93">
         <v>30</v>
       </c>
+      <c r="Q93" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="2">
@@ -6251,6 +6533,9 @@
       </c>
       <c r="P94">
         <v>30</v>
+      </c>
+      <c r="Q94" s="2">
+        <v>43668</v>
       </c>
     </row>
     <row r="95">
@@ -6313,6 +6598,9 @@
       <c r="P95">
         <v>30</v>
       </c>
+      <c r="Q95" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="2">
@@ -6373,6 +6661,9 @@
       <c r="P96">
         <v>30</v>
       </c>
+      <c r="Q96" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="2">
@@ -6429,6 +6720,9 @@
       </c>
       <c r="P97">
         <v>30</v>
+      </c>
+      <c r="Q97" s="2">
+        <v>43668</v>
       </c>
     </row>
     <row r="98">
@@ -6491,6 +6785,9 @@
       <c r="P98">
         <v>30</v>
       </c>
+      <c r="Q98" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="2">
@@ -6554,6 +6851,9 @@
       <c r="P99">
         <v>30</v>
       </c>
+      <c r="Q99" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="2">
@@ -6614,6 +6914,9 @@
       <c r="P100">
         <v>30</v>
       </c>
+      <c r="Q100" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="2">
@@ -6674,6 +6977,9 @@
       <c r="P101">
         <v>30</v>
       </c>
+      <c r="Q101" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="2">
@@ -6732,6 +7038,9 @@
       </c>
       <c r="P102">
         <v>30</v>
+      </c>
+      <c r="Q102" s="2">
+        <v>43668</v>
       </c>
     </row>
     <row r="103">
@@ -6794,6 +7103,9 @@
       <c r="P103">
         <v>30</v>
       </c>
+      <c r="Q103" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="2">
@@ -6852,6 +7164,9 @@
       </c>
       <c r="P104">
         <v>30</v>
+      </c>
+      <c r="Q104" s="2">
+        <v>43668</v>
       </c>
     </row>
     <row r="105">
@@ -6915,6 +7230,9 @@
       <c r="P105">
         <v>30</v>
       </c>
+      <c r="Q105" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="2">
@@ -6976,6 +7294,9 @@
       <c r="P106">
         <v>30</v>
       </c>
+      <c r="Q106" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="2">
@@ -7037,6 +7358,9 @@
       <c r="P107">
         <v>30</v>
       </c>
+      <c r="Q107" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="2">
@@ -7093,6 +7417,9 @@
       <c r="P108">
         <v>30</v>
       </c>
+      <c r="Q108" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="2">
@@ -7148,6 +7475,9 @@
       <c r="P109">
         <v>30</v>
       </c>
+      <c r="Q109" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="2">
@@ -7208,6 +7538,9 @@
       <c r="P110">
         <v>30</v>
       </c>
+      <c r="Q110" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="2">
@@ -7268,6 +7601,9 @@
       <c r="P111">
         <v>30</v>
       </c>
+      <c r="Q111" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="2">
@@ -7328,6 +7664,9 @@
       <c r="P112">
         <v>30</v>
       </c>
+      <c r="Q112" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="2">
@@ -7384,6 +7723,9 @@
       </c>
       <c r="P113">
         <v>30</v>
+      </c>
+      <c r="Q113" s="2">
+        <v>43668</v>
       </c>
     </row>
     <row r="114">
@@ -7446,6 +7788,9 @@
       <c r="P114">
         <v>30</v>
       </c>
+      <c r="Q114" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="2">
@@ -7507,6 +7852,9 @@
       <c r="P115">
         <v>30</v>
       </c>
+      <c r="Q115" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="2">
@@ -7568,6 +7916,9 @@
       <c r="P116">
         <v>30</v>
       </c>
+      <c r="Q116" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="2">
@@ -7627,6 +7978,9 @@
       <c r="P117">
         <v>30</v>
       </c>
+      <c r="Q117" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="2">
@@ -7686,6 +8040,9 @@
       <c r="P118">
         <v>30</v>
       </c>
+      <c r="Q118" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="2">
@@ -7745,6 +8102,9 @@
       <c r="P119">
         <v>30</v>
       </c>
+      <c r="Q119" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="2">
@@ -7801,6 +8161,9 @@
       </c>
       <c r="P120">
         <v>30</v>
+      </c>
+      <c r="Q120" s="2">
+        <v>43668</v>
       </c>
     </row>
     <row r="121">
@@ -7866,6 +8229,9 @@
       <c r="P121">
         <v>30</v>
       </c>
+      <c r="Q121" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="2">
@@ -7925,6 +8291,9 @@
       <c r="P122">
         <v>30</v>
       </c>
+      <c r="Q122" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="2">
@@ -7981,6 +8350,9 @@
       </c>
       <c r="P123">
         <v>30</v>
+      </c>
+      <c r="Q123" s="2">
+        <v>43668</v>
       </c>
     </row>
     <row r="124">
@@ -8043,6 +8415,9 @@
       <c r="P124">
         <v>30</v>
       </c>
+      <c r="Q124" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="2">
@@ -8100,6 +8475,9 @@
       <c r="P125">
         <v>30</v>
       </c>
+      <c r="Q125" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="2">
@@ -8159,6 +8537,9 @@
       <c r="P126">
         <v>30</v>
       </c>
+      <c r="Q126" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="2">
@@ -8217,6 +8598,9 @@
       </c>
       <c r="P127">
         <v>30</v>
+      </c>
+      <c r="Q127" s="2">
+        <v>43668</v>
       </c>
     </row>
     <row r="128">
@@ -8279,6 +8663,9 @@
       <c r="P128">
         <v>30</v>
       </c>
+      <c r="Q128" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" s="2">
@@ -8339,6 +8726,9 @@
       <c r="P129">
         <v>30</v>
       </c>
+      <c r="Q129" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="2">
@@ -8398,6 +8788,9 @@
       </c>
       <c r="P130">
         <v>30</v>
+      </c>
+      <c r="Q130" s="2">
+        <v>43668</v>
       </c>
     </row>
     <row r="131">
@@ -8460,6 +8853,9 @@
       <c r="P131">
         <v>30</v>
       </c>
+      <c r="Q131" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="2">
@@ -8519,6 +8915,9 @@
       </c>
       <c r="P132">
         <v>30</v>
+      </c>
+      <c r="Q132" s="2">
+        <v>43668</v>
       </c>
     </row>
     <row r="133">
@@ -8579,6 +8978,9 @@
       <c r="P133">
         <v>30</v>
       </c>
+      <c r="Q133" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" s="2">
@@ -8632,6 +9034,9 @@
       </c>
       <c r="P134">
         <v>30</v>
+      </c>
+      <c r="Q134" s="2">
+        <v>43668</v>
       </c>
     </row>
     <row r="135">
@@ -8688,6 +9093,9 @@
       <c r="P135">
         <v>30</v>
       </c>
+      <c r="Q135" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" s="2">
@@ -8740,6 +9148,9 @@
       <c r="P136">
         <v>30</v>
       </c>
+      <c r="Q136" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" s="2">
@@ -8794,6 +9205,9 @@
       <c r="P137">
         <v>30</v>
       </c>
+      <c r="Q137" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" s="2">
@@ -8847,6 +9261,9 @@
       </c>
       <c r="P138">
         <v>30</v>
+      </c>
+      <c r="Q138" s="2">
+        <v>43668</v>
       </c>
     </row>
     <row r="139">
@@ -8904,6 +9321,9 @@
       <c r="P139">
         <v>30</v>
       </c>
+      <c r="Q139" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" s="2">
@@ -8958,6 +9378,9 @@
       </c>
       <c r="P140">
         <v>30</v>
+      </c>
+      <c r="Q140" s="2">
+        <v>43668</v>
       </c>
     </row>
     <row r="141">
@@ -9014,6 +9437,9 @@
       </c>
       <c r="P141">
         <v>30</v>
+      </c>
+      <c r="Q141" s="2">
+        <v>43668</v>
       </c>
     </row>
     <row r="142">
@@ -9071,6 +9497,9 @@
       </c>
       <c r="P142">
         <v>30</v>
+      </c>
+      <c r="Q142" s="2">
+        <v>43668</v>
       </c>
     </row>
     <row r="143">
@@ -9133,6 +9562,9 @@
       <c r="P143">
         <v>30</v>
       </c>
+      <c r="Q143" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" s="2">
@@ -9190,6 +9622,9 @@
       <c r="P144">
         <v>30</v>
       </c>
+      <c r="Q144" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" s="2">
@@ -9247,6 +9682,9 @@
       <c r="P145">
         <v>30</v>
       </c>
+      <c r="Q145" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" s="2">
@@ -9308,6 +9746,9 @@
       <c r="P146">
         <v>30</v>
       </c>
+      <c r="Q146" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" s="2">
@@ -9368,6 +9809,9 @@
       <c r="P147">
         <v>30</v>
       </c>
+      <c r="Q147" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" s="2">
@@ -9427,6 +9871,9 @@
       <c r="P148">
         <v>30</v>
       </c>
+      <c r="Q148" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" s="2">
@@ -9484,6 +9931,9 @@
       <c r="P149">
         <v>30</v>
       </c>
+      <c r="Q149" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" s="2">
@@ -9542,6 +9992,9 @@
       </c>
       <c r="P150">
         <v>30</v>
+      </c>
+      <c r="Q150" s="2">
+        <v>43668</v>
       </c>
     </row>
     <row r="151">
@@ -9603,6 +10056,9 @@
       <c r="P151">
         <v>30</v>
       </c>
+      <c r="Q151" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" s="2">
@@ -9662,6 +10118,9 @@
       </c>
       <c r="P152">
         <v>30</v>
+      </c>
+      <c r="Q152" s="2">
+        <v>43668</v>
       </c>
     </row>
     <row r="153">
@@ -9724,6 +10183,9 @@
       <c r="P153">
         <v>30</v>
       </c>
+      <c r="Q153" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" s="2">
@@ -9783,6 +10245,9 @@
       <c r="P154">
         <v>30</v>
       </c>
+      <c r="Q154" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" s="2">
@@ -9842,6 +10307,9 @@
       <c r="P155">
         <v>30</v>
       </c>
+      <c r="Q155" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" s="2">
@@ -9898,6 +10366,9 @@
       </c>
       <c r="P156">
         <v>30</v>
+      </c>
+      <c r="Q156" s="2">
+        <v>43668</v>
       </c>
     </row>
     <row r="157">
@@ -9960,6 +10431,9 @@
       <c r="P157">
         <v>30</v>
       </c>
+      <c r="Q157" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" s="2">
@@ -10020,6 +10494,9 @@
       <c r="P158">
         <v>30</v>
       </c>
+      <c r="Q158" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" s="2">
@@ -10079,6 +10556,9 @@
       <c r="P159">
         <v>30</v>
       </c>
+      <c r="Q159" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" s="2">
@@ -10137,6 +10617,9 @@
       </c>
       <c r="P160">
         <v>30</v>
+      </c>
+      <c r="Q160" s="2">
+        <v>43668</v>
       </c>
     </row>
     <row r="161">
@@ -10198,6 +10681,9 @@
       <c r="P161">
         <v>30</v>
       </c>
+      <c r="Q161" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" s="2">
@@ -10258,6 +10744,9 @@
       <c r="P162">
         <v>30</v>
       </c>
+      <c r="Q162" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" s="2">
@@ -10316,6 +10805,9 @@
       </c>
       <c r="P163">
         <v>30</v>
+      </c>
+      <c r="Q163" s="2">
+        <v>43668</v>
       </c>
     </row>
     <row r="164">
@@ -10378,6 +10870,9 @@
       <c r="P164">
         <v>30</v>
       </c>
+      <c r="Q164" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" s="2">
@@ -10438,6 +10933,9 @@
       <c r="P165">
         <v>30</v>
       </c>
+      <c r="Q165" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" s="2">
@@ -10498,6 +10996,9 @@
       <c r="P166">
         <v>30</v>
       </c>
+      <c r="Q166" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" s="2">
@@ -10557,6 +11058,9 @@
       <c r="P167">
         <v>30</v>
       </c>
+      <c r="Q167" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" s="2">
@@ -10611,6 +11115,9 @@
       <c r="P168">
         <v>30</v>
       </c>
+      <c r="Q168" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" s="2">
@@ -10664,6 +11171,9 @@
       </c>
       <c r="P169">
         <v>30</v>
+      </c>
+      <c r="Q169" s="2">
+        <v>43668</v>
       </c>
     </row>
     <row r="170">
@@ -10720,6 +11230,9 @@
       <c r="P170">
         <v>30</v>
       </c>
+      <c r="Q170" s="2">
+        <v>43668</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" s="2">
@@ -10773,6 +11286,9 @@
       </c>
       <c r="P171">
         <v>30</v>
+      </c>
+      <c r="Q171" s="2">
+        <v>43668</v>
       </c>
     </row>
     <row r="172">
@@ -10830,6 +11346,9 @@
       <c r="P172">
         <v>31</v>
       </c>
+      <c r="Q172" s="2">
+        <v>43675</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" s="2">
@@ -10886,6 +11405,9 @@
       <c r="P173">
         <v>31</v>
       </c>
+      <c r="Q173" s="2">
+        <v>43675</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" s="2">
@@ -10941,6 +11463,9 @@
       <c r="P174">
         <v>31</v>
       </c>
+      <c r="Q174" s="2">
+        <v>43675</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" s="2">
@@ -10995,6 +11520,9 @@
       </c>
       <c r="P175">
         <v>31</v>
+      </c>
+      <c r="Q175" s="2">
+        <v>43675</v>
       </c>
     </row>
     <row r="176">
@@ -11052,6 +11580,9 @@
       <c r="P176">
         <v>31</v>
       </c>
+      <c r="Q176" s="2">
+        <v>43675</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" s="2">
@@ -11105,6 +11636,9 @@
       </c>
       <c r="P177">
         <v>31</v>
+      </c>
+      <c r="Q177" s="2">
+        <v>43675</v>
       </c>
     </row>
     <row r="178">
@@ -11161,6 +11695,9 @@
       </c>
       <c r="P178">
         <v>31</v>
+      </c>
+      <c r="Q178" s="2">
+        <v>43675</v>
       </c>
     </row>
     <row r="179">
@@ -11219,6 +11756,9 @@
       <c r="P179">
         <v>31</v>
       </c>
+      <c r="Q179" s="2">
+        <v>43675</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" s="2">
@@ -11279,6 +11819,9 @@
       <c r="P180">
         <v>31</v>
       </c>
+      <c r="Q180" s="2">
+        <v>43675</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" s="2">
@@ -11333,6 +11876,9 @@
       </c>
       <c r="P181">
         <v>31</v>
+      </c>
+      <c r="Q181" s="2">
+        <v>43675</v>
       </c>
     </row>
     <row r="182">
@@ -11392,6 +11938,9 @@
       <c r="P182">
         <v>31</v>
       </c>
+      <c r="Q182" s="2">
+        <v>43675</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" s="2">
@@ -11449,6 +11998,9 @@
       <c r="P183">
         <v>31</v>
       </c>
+      <c r="Q183" s="2">
+        <v>43675</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184" s="2">
@@ -11504,6 +12056,9 @@
       <c r="P184">
         <v>31</v>
       </c>
+      <c r="Q184" s="2">
+        <v>43675</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185" s="2">
@@ -11557,6 +12112,9 @@
       <c r="P185">
         <v>31</v>
       </c>
+      <c r="Q185" s="2">
+        <v>43675</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" s="2">
@@ -11609,6 +12167,9 @@
       </c>
       <c r="P186">
         <v>31</v>
+      </c>
+      <c r="Q186" s="2">
+        <v>43675</v>
       </c>
     </row>
     <row r="187">
@@ -11664,6 +12225,9 @@
       </c>
       <c r="P187">
         <v>31</v>
+      </c>
+      <c r="Q187" s="2">
+        <v>43675</v>
       </c>
     </row>
     <row r="188">
@@ -11722,6 +12286,9 @@
       <c r="P188">
         <v>31</v>
       </c>
+      <c r="Q188" s="2">
+        <v>43675</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" s="2">
@@ -11775,6 +12342,9 @@
       </c>
       <c r="P189">
         <v>31</v>
+      </c>
+      <c r="Q189" s="2">
+        <v>43675</v>
       </c>
     </row>
     <row r="190">
@@ -11830,6 +12400,9 @@
       </c>
       <c r="P190">
         <v>31</v>
+      </c>
+      <c r="Q190" s="2">
+        <v>43675</v>
       </c>
     </row>
     <row r="191">
@@ -11887,6 +12460,9 @@
       </c>
       <c r="P191">
         <v>31</v>
+      </c>
+      <c r="Q191" s="2">
+        <v>43675</v>
       </c>
     </row>
     <row r="192">
@@ -11946,6 +12522,9 @@
       <c r="P192">
         <v>31</v>
       </c>
+      <c r="Q192" s="2">
+        <v>43675</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" s="2">
@@ -12010,6 +12589,9 @@
       </c>
       <c r="P193">
         <v>31</v>
+      </c>
+      <c r="Q193" s="2">
+        <v>43675</v>
       </c>
     </row>
     <row r="194">
@@ -12078,6 +12660,9 @@
       <c r="P194">
         <v>31</v>
       </c>
+      <c r="Q194" s="2">
+        <v>43675</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" s="2">
@@ -12142,6 +12727,9 @@
       <c r="P195">
         <v>31</v>
       </c>
+      <c r="Q195" s="2">
+        <v>43675</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" s="2">
@@ -12206,6 +12794,9 @@
       <c r="P196">
         <v>31</v>
       </c>
+      <c r="Q196" s="2">
+        <v>43675</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" s="2">
@@ -12270,6 +12861,9 @@
       <c r="P197">
         <v>31</v>
       </c>
+      <c r="Q197" s="2">
+        <v>43675</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198" s="2">
@@ -12333,6 +12927,9 @@
       </c>
       <c r="P198">
         <v>31</v>
+      </c>
+      <c r="Q198" s="2">
+        <v>43675</v>
       </c>
     </row>
     <row r="199">
@@ -12401,6 +12998,9 @@
       <c r="P199">
         <v>31</v>
       </c>
+      <c r="Q199" s="2">
+        <v>43675</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" s="2">
@@ -12464,6 +13064,9 @@
       </c>
       <c r="P200">
         <v>31</v>
+      </c>
+      <c r="Q200" s="2">
+        <v>43675</v>
       </c>
     </row>
     <row r="201">
@@ -12530,6 +13133,9 @@
       <c r="P201">
         <v>31</v>
       </c>
+      <c r="Q201" s="2">
+        <v>43675</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" s="2">
@@ -12594,6 +13200,9 @@
       <c r="P202">
         <v>31</v>
       </c>
+      <c r="Q202" s="2">
+        <v>43675</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" s="2">
@@ -12658,6 +13267,9 @@
       <c r="P203">
         <v>31</v>
       </c>
+      <c r="Q203" s="2">
+        <v>43675</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" s="2">
@@ -12722,6 +13334,9 @@
       <c r="P204">
         <v>31</v>
       </c>
+      <c r="Q204" s="2">
+        <v>43675</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205" s="2">
@@ -12786,6 +13401,9 @@
       <c r="P205">
         <v>31</v>
       </c>
+      <c r="Q205" s="2">
+        <v>43675</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206" s="2">
@@ -12849,6 +13467,9 @@
       </c>
       <c r="P206">
         <v>31</v>
+      </c>
+      <c r="Q206" s="2">
+        <v>43675</v>
       </c>
     </row>
     <row r="207">
@@ -12915,6 +13536,9 @@
       </c>
       <c r="P207">
         <v>31</v>
+      </c>
+      <c r="Q207" s="2">
+        <v>43675</v>
       </c>
     </row>
     <row r="208">
@@ -12984,6 +13608,9 @@
       <c r="P208">
         <v>31</v>
       </c>
+      <c r="Q208" s="2">
+        <v>43675</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209" s="2">
@@ -13050,6 +13677,9 @@
       <c r="P209">
         <v>31</v>
       </c>
+      <c r="Q209" s="2">
+        <v>43675</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" s="2">
@@ -13114,6 +13744,9 @@
       <c r="P210">
         <v>31</v>
       </c>
+      <c r="Q210" s="2">
+        <v>43675</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" s="2">
@@ -13178,6 +13811,9 @@
       <c r="P211">
         <v>31</v>
       </c>
+      <c r="Q211" s="2">
+        <v>43675</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212" s="2">
@@ -13242,6 +13878,9 @@
       <c r="P212">
         <v>31</v>
       </c>
+      <c r="Q212" s="2">
+        <v>43675</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213" s="2">
@@ -13304,6 +13943,9 @@
       <c r="P213">
         <v>31</v>
       </c>
+      <c r="Q213" s="2">
+        <v>43675</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214" s="2">
@@ -13367,6 +14009,9 @@
       </c>
       <c r="P214">
         <v>31</v>
+      </c>
+      <c r="Q214" s="2">
+        <v>43675</v>
       </c>
     </row>
     <row r="215">
@@ -13432,6 +14077,9 @@
       </c>
       <c r="P215">
         <v>31</v>
+      </c>
+      <c r="Q215" s="2">
+        <v>43675</v>
       </c>
     </row>
     <row r="216">
@@ -13501,6 +14149,9 @@
       <c r="P216">
         <v>31</v>
       </c>
+      <c r="Q216" s="2">
+        <v>43675</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217" s="2">
@@ -13564,6 +14215,9 @@
       </c>
       <c r="P217">
         <v>31</v>
+      </c>
+      <c r="Q217" s="2">
+        <v>43675</v>
       </c>
     </row>
     <row r="218">
@@ -13627,6 +14281,9 @@
       <c r="P218">
         <v>31</v>
       </c>
+      <c r="Q218" s="2">
+        <v>43675</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" s="2">
@@ -13692,6 +14349,9 @@
       </c>
       <c r="P219">
         <v>31</v>
+      </c>
+      <c r="Q219" s="2">
+        <v>43675</v>
       </c>
     </row>
     <row r="220">
@@ -13751,6 +14411,9 @@
       <c r="P220">
         <v>31</v>
       </c>
+      <c r="Q220" s="2">
+        <v>43675</v>
+      </c>
     </row>
     <row r="221">
       <c r="A221" s="2">
@@ -13804,6 +14467,9 @@
       <c r="P221">
         <v>31</v>
       </c>
+      <c r="Q221" s="2">
+        <v>43675</v>
+      </c>
     </row>
     <row r="222">
       <c r="A222" s="2">
@@ -13858,6 +14524,9 @@
       <c r="P222">
         <v>31</v>
       </c>
+      <c r="Q222" s="2">
+        <v>43675</v>
+      </c>
     </row>
     <row r="223">
       <c r="A223" s="2">
@@ -13916,6 +14585,9 @@
       <c r="P223">
         <v>31</v>
       </c>
+      <c r="Q223" s="2">
+        <v>43675</v>
+      </c>
     </row>
     <row r="224">
       <c r="A224" s="2">
@@ -13967,6 +14639,9 @@
       </c>
       <c r="P224">
         <v>31</v>
+      </c>
+      <c r="Q224" s="2">
+        <v>43675</v>
       </c>
     </row>
     <row r="225">
@@ -14023,6 +14698,9 @@
       </c>
       <c r="P225">
         <v>31</v>
+      </c>
+      <c r="Q225" s="2">
+        <v>43675</v>
       </c>
     </row>
     <row r="226">
@@ -14082,6 +14760,9 @@
       <c r="P226">
         <v>31</v>
       </c>
+      <c r="Q226" s="2">
+        <v>43675</v>
+      </c>
     </row>
     <row r="227">
       <c r="A227" s="2">
@@ -14135,6 +14816,9 @@
       </c>
       <c r="P227">
         <v>31</v>
+      </c>
+      <c r="Q227" s="2">
+        <v>43675</v>
       </c>
     </row>
     <row r="228">
@@ -14192,6 +14876,9 @@
       <c r="P228">
         <v>32</v>
       </c>
+      <c r="Q228" s="2">
+        <v>43682</v>
+      </c>
     </row>
     <row r="229">
       <c r="A229" s="2">
@@ -14247,6 +14934,9 @@
       <c r="P229">
         <v>32</v>
       </c>
+      <c r="Q229" s="2">
+        <v>43682</v>
+      </c>
     </row>
     <row r="230">
       <c r="A230" s="2">
@@ -14300,6 +14990,9 @@
       <c r="P230">
         <v>32</v>
       </c>
+      <c r="Q230" s="2">
+        <v>43682</v>
+      </c>
     </row>
     <row r="231">
       <c r="A231" s="2">
@@ -14351,6 +15044,9 @@
       </c>
       <c r="P231">
         <v>32</v>
+      </c>
+      <c r="Q231" s="2">
+        <v>43682</v>
       </c>
     </row>
     <row r="232">
@@ -14408,6 +15104,9 @@
       <c r="P232">
         <v>32</v>
       </c>
+      <c r="Q232" s="2">
+        <v>43682</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233" s="2">
@@ -14483,6 +15182,9 @@
       <c r="P233">
         <v>32</v>
       </c>
+      <c r="Q233" s="2">
+        <v>43682</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234" s="2">
@@ -14545,6 +15247,9 @@
       </c>
       <c r="P234">
         <v>32</v>
+      </c>
+      <c r="Q234" s="2">
+        <v>43682</v>
       </c>
     </row>
     <row r="235">
@@ -14612,6 +15317,9 @@
       <c r="P235">
         <v>32</v>
       </c>
+      <c r="Q235" s="2">
+        <v>43682</v>
+      </c>
     </row>
     <row r="236">
       <c r="A236" s="2">
@@ -14666,6 +15374,9 @@
       <c r="P236">
         <v>32</v>
       </c>
+      <c r="Q236" s="2">
+        <v>43682</v>
+      </c>
     </row>
     <row r="237">
       <c r="A237" s="2">
@@ -14718,6 +15429,9 @@
       </c>
       <c r="P237">
         <v>32</v>
+      </c>
+      <c r="Q237" s="2">
+        <v>43682</v>
       </c>
     </row>
     <row r="238">
@@ -14784,6 +15498,9 @@
       <c r="P238">
         <v>32</v>
       </c>
+      <c r="Q238" s="2">
+        <v>43682</v>
+      </c>
     </row>
     <row r="239">
       <c r="A239" s="2">
@@ -14837,6 +15554,9 @@
       <c r="P239">
         <v>32</v>
       </c>
+      <c r="Q239" s="2">
+        <v>43682</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240" s="2">
@@ -14891,6 +15611,9 @@
       <c r="P240">
         <v>32</v>
       </c>
+      <c r="Q240" s="2">
+        <v>43682</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241" s="2">
@@ -14944,6 +15667,9 @@
       <c r="P241">
         <v>32</v>
       </c>
+      <c r="Q241" s="2">
+        <v>43682</v>
+      </c>
     </row>
     <row r="242">
       <c r="A242" s="2">
@@ -14996,6 +15722,9 @@
       <c r="P242">
         <v>32</v>
       </c>
+      <c r="Q242" s="2">
+        <v>43682</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243" s="2">
@@ -15050,6 +15779,9 @@
       <c r="P243">
         <v>32</v>
       </c>
+      <c r="Q243" s="2">
+        <v>43682</v>
+      </c>
     </row>
     <row r="244">
       <c r="A244" s="2">
@@ -15104,6 +15836,9 @@
       <c r="P244">
         <v>32</v>
       </c>
+      <c r="Q244" s="2">
+        <v>43682</v>
+      </c>
     </row>
     <row r="245">
       <c r="A245" s="2">
@@ -15158,6 +15893,9 @@
       <c r="P245">
         <v>32</v>
       </c>
+      <c r="Q245" s="2">
+        <v>43682</v>
+      </c>
     </row>
     <row r="246">
       <c r="A246" s="2">
@@ -15210,6 +15948,9 @@
       </c>
       <c r="P246">
         <v>32</v>
+      </c>
+      <c r="Q246" s="2">
+        <v>43682</v>
       </c>
     </row>
     <row r="247">
@@ -15267,6 +16008,9 @@
       <c r="P247">
         <v>32</v>
       </c>
+      <c r="Q247" s="2">
+        <v>43682</v>
+      </c>
     </row>
     <row r="248">
       <c r="A248" s="2">
@@ -15319,6 +16063,9 @@
       </c>
       <c r="P248">
         <v>32</v>
+      </c>
+      <c r="Q248" s="2">
+        <v>43682</v>
       </c>
     </row>
     <row r="249">
@@ -15377,6 +16124,9 @@
       <c r="P249">
         <v>33</v>
       </c>
+      <c r="Q249" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="250">
       <c r="A250" s="2">
@@ -15431,6 +16181,9 @@
       <c r="P250">
         <v>33</v>
       </c>
+      <c r="Q250" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="251">
       <c r="A251" s="2">
@@ -15484,6 +16237,9 @@
       </c>
       <c r="P251">
         <v>33</v>
+      </c>
+      <c r="Q251" s="2">
+        <v>43689</v>
       </c>
     </row>
     <row r="252">
@@ -15550,6 +16306,9 @@
       <c r="P252">
         <v>33</v>
       </c>
+      <c r="Q252" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="253">
       <c r="A253" s="2">
@@ -15614,6 +16373,9 @@
       <c r="P253">
         <v>33</v>
       </c>
+      <c r="Q253" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="254">
       <c r="A254" s="2">
@@ -15678,6 +16440,9 @@
       <c r="P254">
         <v>33</v>
       </c>
+      <c r="Q254" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="255">
       <c r="A255" s="2">
@@ -15742,6 +16507,9 @@
       <c r="P255">
         <v>33</v>
       </c>
+      <c r="Q255" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="256">
       <c r="A256" s="2">
@@ -15806,6 +16574,9 @@
       <c r="P256">
         <v>33</v>
       </c>
+      <c r="Q256" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="257">
       <c r="A257" s="2">
@@ -15869,6 +16640,9 @@
       </c>
       <c r="P257">
         <v>33</v>
+      </c>
+      <c r="Q257" s="2">
+        <v>43689</v>
       </c>
     </row>
     <row r="258">
@@ -15935,6 +16709,9 @@
       <c r="P258">
         <v>33</v>
       </c>
+      <c r="Q258" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="259">
       <c r="A259" s="2">
@@ -16010,6 +16787,9 @@
       <c r="P259">
         <v>33</v>
       </c>
+      <c r="Q259" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="260">
       <c r="A260" s="2">
@@ -16074,6 +16854,9 @@
       <c r="P260">
         <v>33</v>
       </c>
+      <c r="Q260" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="261">
       <c r="A261" s="2">
@@ -16136,6 +16919,9 @@
       </c>
       <c r="P261">
         <v>33</v>
+      </c>
+      <c r="Q261" s="2">
+        <v>43689</v>
       </c>
     </row>
     <row r="262">
@@ -16202,6 +16988,9 @@
       <c r="P262">
         <v>33</v>
       </c>
+      <c r="Q262" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="263">
       <c r="A263" s="2">
@@ -16266,6 +17055,9 @@
       <c r="P263">
         <v>33</v>
       </c>
+      <c r="Q263" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="264">
       <c r="A264" s="2">
@@ -16328,6 +17120,9 @@
       <c r="P264">
         <v>33</v>
       </c>
+      <c r="Q264" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="265">
       <c r="A265" s="2">
@@ -16391,6 +17186,9 @@
       <c r="P265">
         <v>33</v>
       </c>
+      <c r="Q265" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="266">
       <c r="A266" s="2">
@@ -16454,6 +17252,9 @@
       <c r="P266">
         <v>33</v>
       </c>
+      <c r="Q266" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="267">
       <c r="A267" s="2">
@@ -16516,6 +17317,9 @@
       <c r="P267">
         <v>33</v>
       </c>
+      <c r="Q267" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="268">
       <c r="A268" s="2">
@@ -16577,6 +17381,9 @@
       </c>
       <c r="P268">
         <v>33</v>
+      </c>
+      <c r="Q268" s="2">
+        <v>43689</v>
       </c>
     </row>
     <row r="269">
@@ -16643,6 +17450,9 @@
       <c r="P269">
         <v>33</v>
       </c>
+      <c r="Q269" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="270">
       <c r="A270" s="2">
@@ -16704,6 +17514,9 @@
       </c>
       <c r="P270">
         <v>33</v>
+      </c>
+      <c r="Q270" s="2">
+        <v>43689</v>
       </c>
     </row>
     <row r="271">
@@ -16770,6 +17583,9 @@
       <c r="P271">
         <v>33</v>
       </c>
+      <c r="Q271" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="272">
       <c r="A272" s="2">
@@ -16834,6 +17650,9 @@
       <c r="P272">
         <v>33</v>
       </c>
+      <c r="Q272" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="273">
       <c r="A273" s="2">
@@ -16898,6 +17717,9 @@
       <c r="P273">
         <v>33</v>
       </c>
+      <c r="Q273" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="274">
       <c r="A274" s="2">
@@ -16962,6 +17784,9 @@
       <c r="P274">
         <v>33</v>
       </c>
+      <c r="Q274" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="275">
       <c r="A275" s="2">
@@ -17025,6 +17850,9 @@
       </c>
       <c r="P275">
         <v>33</v>
+      </c>
+      <c r="Q275" s="2">
+        <v>43689</v>
       </c>
     </row>
     <row r="276">
@@ -17090,6 +17918,9 @@
       </c>
       <c r="P276">
         <v>33</v>
+      </c>
+      <c r="Q276" s="2">
+        <v>43689</v>
       </c>
     </row>
     <row r="277">
@@ -17156,6 +17987,9 @@
       </c>
       <c r="P277">
         <v>33</v>
+      </c>
+      <c r="Q277" s="2">
+        <v>43689</v>
       </c>
     </row>
     <row r="278">
@@ -17214,6 +18048,9 @@
       <c r="P278">
         <v>33</v>
       </c>
+      <c r="Q278" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="279">
       <c r="A279" s="2">
@@ -17271,6 +18108,9 @@
       <c r="P279">
         <v>33</v>
       </c>
+      <c r="Q279" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="280">
       <c r="A280" s="2">
@@ -17328,6 +18168,9 @@
       <c r="P280">
         <v>33</v>
       </c>
+      <c r="Q280" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="281">
       <c r="A281" s="2">
@@ -17380,6 +18223,9 @@
       </c>
       <c r="P281">
         <v>33</v>
+      </c>
+      <c r="Q281" s="2">
+        <v>43689</v>
       </c>
     </row>
     <row r="282">
@@ -17438,6 +18284,9 @@
       <c r="P282">
         <v>33</v>
       </c>
+      <c r="Q282" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="283">
       <c r="A283" s="2">
@@ -17490,6 +18339,9 @@
       <c r="P283">
         <v>33</v>
       </c>
+      <c r="Q283" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="284">
       <c r="A284" s="2">
@@ -17543,6 +18395,9 @@
       <c r="P284">
         <v>33</v>
       </c>
+      <c r="Q284" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="285">
       <c r="A285" s="2">
@@ -17596,6 +18451,9 @@
       <c r="P285">
         <v>33</v>
       </c>
+      <c r="Q285" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="286">
       <c r="A286" s="2">
@@ -17650,6 +18508,9 @@
       <c r="P286">
         <v>33</v>
       </c>
+      <c r="Q286" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="287">
       <c r="A287" s="2">
@@ -17703,6 +18564,9 @@
       <c r="P287">
         <v>33</v>
       </c>
+      <c r="Q287" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="288">
       <c r="A288" s="2">
@@ -17756,6 +18620,9 @@
       </c>
       <c r="P288">
         <v>33</v>
+      </c>
+      <c r="Q288" s="2">
+        <v>43689</v>
       </c>
     </row>
     <row r="289">
@@ -17813,6 +18680,9 @@
       <c r="P289">
         <v>33</v>
       </c>
+      <c r="Q289" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="290">
       <c r="A290" s="2">
@@ -17876,6 +18746,9 @@
       </c>
       <c r="P290">
         <v>33</v>
+      </c>
+      <c r="Q290" s="2">
+        <v>43689</v>
       </c>
     </row>
     <row r="291">
@@ -17952,6 +18825,9 @@
       <c r="P291">
         <v>33</v>
       </c>
+      <c r="Q291" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="292">
       <c r="A292" s="2">
@@ -18016,6 +18892,9 @@
       <c r="P292">
         <v>33</v>
       </c>
+      <c r="Q292" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="293">
       <c r="A293" s="2">
@@ -18080,6 +18959,9 @@
       <c r="P293">
         <v>33</v>
       </c>
+      <c r="Q293" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="294">
       <c r="A294" s="2">
@@ -18144,6 +19026,9 @@
       <c r="P294">
         <v>33</v>
       </c>
+      <c r="Q294" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="295">
       <c r="A295" s="2">
@@ -18208,6 +19093,9 @@
       <c r="P295">
         <v>33</v>
       </c>
+      <c r="Q295" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="296">
       <c r="A296" s="2">
@@ -18281,6 +19169,9 @@
       <c r="P296">
         <v>33</v>
       </c>
+      <c r="Q296" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="297">
       <c r="A297" s="2">
@@ -18343,6 +19234,9 @@
       <c r="P297">
         <v>33</v>
       </c>
+      <c r="Q297" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="298">
       <c r="A298" s="2">
@@ -18406,6 +19300,9 @@
       <c r="P298">
         <v>33</v>
       </c>
+      <c r="Q298" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="299">
       <c r="A299" s="2">
@@ -18469,6 +19366,9 @@
       </c>
       <c r="P299">
         <v>33</v>
+      </c>
+      <c r="Q299" s="2">
+        <v>43689</v>
       </c>
     </row>
     <row r="300">
@@ -18535,6 +19435,9 @@
       <c r="P300">
         <v>33</v>
       </c>
+      <c r="Q300" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="301">
       <c r="A301" s="2">
@@ -18599,6 +19502,9 @@
       <c r="P301">
         <v>33</v>
       </c>
+      <c r="Q301" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="302">
       <c r="A302" s="2">
@@ -18661,6 +19567,9 @@
       <c r="P302">
         <v>33</v>
       </c>
+      <c r="Q302" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="303">
       <c r="A303" s="2">
@@ -18723,6 +19632,9 @@
       </c>
       <c r="P303">
         <v>33</v>
+      </c>
+      <c r="Q303" s="2">
+        <v>43689</v>
       </c>
     </row>
     <row r="304">
@@ -18789,6 +19701,9 @@
       <c r="P304">
         <v>33</v>
       </c>
+      <c r="Q304" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="305">
       <c r="A305" s="2">
@@ -18851,6 +19766,9 @@
       </c>
       <c r="P305">
         <v>33</v>
+      </c>
+      <c r="Q305" s="2">
+        <v>43689</v>
       </c>
     </row>
     <row r="306">
@@ -18920,6 +19838,9 @@
       <c r="P306">
         <v>33</v>
       </c>
+      <c r="Q306" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="307">
       <c r="A307" s="2">
@@ -18984,6 +19905,9 @@
       <c r="P307">
         <v>33</v>
       </c>
+      <c r="Q307" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="308">
       <c r="A308" s="2">
@@ -19048,6 +19972,9 @@
       <c r="P308">
         <v>33</v>
       </c>
+      <c r="Q308" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="309">
       <c r="A309" s="2">
@@ -19110,6 +20037,9 @@
       <c r="P309">
         <v>33</v>
       </c>
+      <c r="Q309" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="310">
       <c r="A310" s="2">
@@ -19172,6 +20102,9 @@
       </c>
       <c r="P310">
         <v>33</v>
+      </c>
+      <c r="Q310" s="2">
+        <v>43689</v>
       </c>
     </row>
     <row r="311">
@@ -19240,6 +20173,9 @@
       <c r="P311">
         <v>33</v>
       </c>
+      <c r="Q311" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="312">
       <c r="A312" s="2">
@@ -19304,6 +20240,9 @@
       <c r="P312">
         <v>33</v>
       </c>
+      <c r="Q312" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="313">
       <c r="A313" s="2">
@@ -19368,6 +20307,9 @@
       <c r="P313">
         <v>33</v>
       </c>
+      <c r="Q313" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="314">
       <c r="A314" s="2">
@@ -19430,6 +20372,9 @@
       </c>
       <c r="P314">
         <v>33</v>
+      </c>
+      <c r="Q314" s="2">
+        <v>43689</v>
       </c>
     </row>
     <row r="315">
@@ -19497,6 +20442,9 @@
       <c r="P315">
         <v>33</v>
       </c>
+      <c r="Q315" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="316">
       <c r="A316" s="2">
@@ -19559,6 +20507,9 @@
       </c>
       <c r="P316">
         <v>33</v>
+      </c>
+      <c r="Q316" s="2">
+        <v>43689</v>
       </c>
     </row>
     <row r="317">
@@ -19616,6 +20567,9 @@
       <c r="P317">
         <v>33</v>
       </c>
+      <c r="Q317" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="318">
       <c r="A318" s="2">
@@ -19668,6 +20622,9 @@
       <c r="P318">
         <v>33</v>
       </c>
+      <c r="Q318" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="319">
       <c r="A319" s="2">
@@ -19727,6 +20684,9 @@
       <c r="P319">
         <v>33</v>
       </c>
+      <c r="Q319" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="320">
       <c r="A320" s="2">
@@ -19780,6 +20740,9 @@
       <c r="P320">
         <v>33</v>
       </c>
+      <c r="Q320" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="321">
       <c r="A321" s="2">
@@ -19834,6 +20797,9 @@
       <c r="P321">
         <v>33</v>
       </c>
+      <c r="Q321" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="322">
       <c r="A322" s="2">
@@ -19887,6 +20853,9 @@
       <c r="P322">
         <v>33</v>
       </c>
+      <c r="Q322" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="323">
       <c r="A323" s="2">
@@ -19940,6 +20909,9 @@
       </c>
       <c r="P323">
         <v>33</v>
+      </c>
+      <c r="Q323" s="2">
+        <v>43689</v>
       </c>
     </row>
     <row r="324">
@@ -19996,6 +20968,9 @@
       <c r="P324">
         <v>33</v>
       </c>
+      <c r="Q324" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="325">
       <c r="A325" s="2">
@@ -20049,6 +21024,9 @@
       <c r="P325">
         <v>33</v>
       </c>
+      <c r="Q325" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="326">
       <c r="A326" s="2">
@@ -20100,6 +21078,9 @@
       </c>
       <c r="P326">
         <v>33</v>
+      </c>
+      <c r="Q326" s="2">
+        <v>43689</v>
       </c>
     </row>
     <row r="327">
@@ -20158,6 +21139,9 @@
       <c r="P327">
         <v>33</v>
       </c>
+      <c r="Q327" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="328">
       <c r="A328" s="2">
@@ -20215,6 +21199,9 @@
       <c r="P328">
         <v>33</v>
       </c>
+      <c r="Q328" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="329">
       <c r="A329" s="2">
@@ -20268,6 +21255,9 @@
       <c r="P329">
         <v>33</v>
       </c>
+      <c r="Q329" s="2">
+        <v>43689</v>
+      </c>
     </row>
     <row r="330">
       <c r="A330" s="2">
@@ -20332,6 +21322,9 @@
       <c r="P330">
         <v>34</v>
       </c>
+      <c r="Q330" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="331">
       <c r="A331" s="2">
@@ -20385,6 +21378,9 @@
       <c r="P331">
         <v>34</v>
       </c>
+      <c r="Q331" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="332">
       <c r="A332" s="2">
@@ -20437,6 +21433,9 @@
       </c>
       <c r="P332">
         <v>34</v>
+      </c>
+      <c r="Q332" s="2">
+        <v>43696</v>
       </c>
     </row>
     <row r="333">
@@ -20494,6 +21493,9 @@
       <c r="P333">
         <v>34</v>
       </c>
+      <c r="Q333" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="334">
       <c r="A334" s="2">
@@ -20548,6 +21550,9 @@
       <c r="P334">
         <v>34</v>
       </c>
+      <c r="Q334" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="335">
       <c r="A335" s="2">
@@ -20601,6 +21606,9 @@
       <c r="P335">
         <v>34</v>
       </c>
+      <c r="Q335" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="336">
       <c r="A336" s="2">
@@ -20654,6 +21662,9 @@
       <c r="P336">
         <v>34</v>
       </c>
+      <c r="Q336" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="337">
       <c r="A337" s="2">
@@ -20707,6 +21718,9 @@
       <c r="P337">
         <v>34</v>
       </c>
+      <c r="Q337" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="338">
       <c r="A338" s="2">
@@ -20760,6 +21774,9 @@
       <c r="P338">
         <v>34</v>
       </c>
+      <c r="Q338" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="339">
       <c r="A339" s="2">
@@ -20812,6 +21829,9 @@
       <c r="P339">
         <v>34</v>
       </c>
+      <c r="Q339" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="340">
       <c r="A340" s="2">
@@ -20866,6 +21886,9 @@
       <c r="P340">
         <v>34</v>
       </c>
+      <c r="Q340" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="341">
       <c r="A341" s="2">
@@ -20918,6 +21941,9 @@
       <c r="P341">
         <v>34</v>
       </c>
+      <c r="Q341" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="342">
       <c r="A342" s="2">
@@ -20972,6 +21998,9 @@
       <c r="P342">
         <v>34</v>
       </c>
+      <c r="Q342" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="343">
       <c r="A343" s="2">
@@ -21025,6 +22054,9 @@
       <c r="P343">
         <v>34</v>
       </c>
+      <c r="Q343" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="344">
       <c r="A344" s="2">
@@ -21078,6 +22110,9 @@
       <c r="P344">
         <v>34</v>
       </c>
+      <c r="Q344" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="345">
       <c r="A345" s="2">
@@ -21130,6 +22165,9 @@
       <c r="P345">
         <v>34</v>
       </c>
+      <c r="Q345" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="346">
       <c r="A346" s="2">
@@ -21184,6 +22222,9 @@
       <c r="P346">
         <v>34</v>
       </c>
+      <c r="Q346" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="347">
       <c r="A347" s="2">
@@ -21248,6 +22289,9 @@
       <c r="P347">
         <v>34</v>
       </c>
+      <c r="Q347" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="348">
       <c r="A348" s="2">
@@ -21301,6 +22345,9 @@
       <c r="P348">
         <v>34</v>
       </c>
+      <c r="Q348" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="349">
       <c r="A349" s="2">
@@ -21355,6 +22402,9 @@
       <c r="P349">
         <v>34</v>
       </c>
+      <c r="Q349" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="350">
       <c r="A350" s="2">
@@ -21407,6 +22457,9 @@
       <c r="P350">
         <v>34</v>
       </c>
+      <c r="Q350" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="351">
       <c r="A351" s="2">
@@ -21459,6 +22512,9 @@
       <c r="P351">
         <v>34</v>
       </c>
+      <c r="Q351" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="352">
       <c r="A352" s="2">
@@ -21511,6 +22567,9 @@
       <c r="P352">
         <v>34</v>
       </c>
+      <c r="Q352" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="353">
       <c r="A353" s="2">
@@ -21563,6 +22622,9 @@
       <c r="P353">
         <v>34</v>
       </c>
+      <c r="Q353" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="354">
       <c r="A354" s="2">
@@ -21615,6 +22677,9 @@
       <c r="P354">
         <v>34</v>
       </c>
+      <c r="Q354" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="355">
       <c r="A355" s="2">
@@ -21678,6 +22743,9 @@
       <c r="P355">
         <v>34</v>
       </c>
+      <c r="Q355" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="356">
       <c r="A356" s="2">
@@ -21741,6 +22809,9 @@
       <c r="P356">
         <v>34</v>
       </c>
+      <c r="Q356" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="357">
       <c r="A357" s="2">
@@ -21804,6 +22875,9 @@
       <c r="P357">
         <v>34</v>
       </c>
+      <c r="Q357" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="358">
       <c r="A358" s="2">
@@ -21867,6 +22941,9 @@
       <c r="P358">
         <v>34</v>
       </c>
+      <c r="Q358" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="359">
       <c r="A359" s="2">
@@ -21930,6 +23007,9 @@
       <c r="P359">
         <v>34</v>
       </c>
+      <c r="Q359" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="360">
       <c r="A360" s="2">
@@ -21983,6 +23063,9 @@
       <c r="P360">
         <v>34</v>
       </c>
+      <c r="Q360" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="361">
       <c r="A361" s="2">
@@ -22035,6 +23118,9 @@
       </c>
       <c r="P361">
         <v>34</v>
+      </c>
+      <c r="Q361" s="2">
+        <v>43696</v>
       </c>
     </row>
     <row r="362">
@@ -22097,6 +23183,9 @@
       <c r="P362">
         <v>34</v>
       </c>
+      <c r="Q362" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="363">
       <c r="A363" s="2">
@@ -22161,6 +23250,9 @@
       <c r="P363">
         <v>34</v>
       </c>
+      <c r="Q363" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="364">
       <c r="A364" s="2">
@@ -22213,6 +23305,9 @@
       <c r="P364">
         <v>34</v>
       </c>
+      <c r="Q364" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="365">
       <c r="A365" s="2">
@@ -22265,6 +23360,9 @@
       </c>
       <c r="P365">
         <v>34</v>
+      </c>
+      <c r="Q365" s="2">
+        <v>43696</v>
       </c>
     </row>
     <row r="366">
@@ -22321,6 +23419,9 @@
       </c>
       <c r="P366">
         <v>34</v>
+      </c>
+      <c r="Q366" s="2">
+        <v>43696</v>
       </c>
     </row>
     <row r="367">
@@ -22380,6 +23481,9 @@
       <c r="P367">
         <v>34</v>
       </c>
+      <c r="Q367" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="368">
       <c r="A368" s="2">
@@ -22432,6 +23536,9 @@
       <c r="P368">
         <v>34</v>
       </c>
+      <c r="Q368" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="369">
       <c r="A369" s="2">
@@ -22491,6 +23598,9 @@
       <c r="P369">
         <v>34</v>
       </c>
+      <c r="Q369" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="370">
       <c r="A370" s="2">
@@ -22543,6 +23653,9 @@
       <c r="P370">
         <v>34</v>
       </c>
+      <c r="Q370" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="371">
       <c r="A371" s="2">
@@ -22596,6 +23709,9 @@
       <c r="P371">
         <v>34</v>
       </c>
+      <c r="Q371" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="372">
       <c r="A372" s="2">
@@ -22648,6 +23764,9 @@
       <c r="P372">
         <v>34</v>
       </c>
+      <c r="Q372" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="373">
       <c r="A373" s="2">
@@ -22702,6 +23821,9 @@
       <c r="P373">
         <v>34</v>
       </c>
+      <c r="Q373" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="374">
       <c r="A374" s="2">
@@ -22754,6 +23876,9 @@
       <c r="P374">
         <v>34</v>
       </c>
+      <c r="Q374" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="375">
       <c r="A375" s="2">
@@ -22806,6 +23931,9 @@
       </c>
       <c r="P375">
         <v>34</v>
+      </c>
+      <c r="Q375" s="2">
+        <v>43696</v>
       </c>
     </row>
     <row r="376">
@@ -22871,6 +23999,9 @@
       </c>
       <c r="P376">
         <v>34</v>
+      </c>
+      <c r="Q376" s="2">
+        <v>43696</v>
       </c>
     </row>
     <row r="377">
@@ -22935,6 +24066,9 @@
       <c r="P377">
         <v>34</v>
       </c>
+      <c r="Q377" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="378">
       <c r="A378" s="2">
@@ -22994,6 +24128,9 @@
       <c r="P378">
         <v>34</v>
       </c>
+      <c r="Q378" s="2">
+        <v>43696</v>
+      </c>
     </row>
     <row r="379">
       <c r="A379" s="2">
@@ -23050,6 +24187,9 @@
       </c>
       <c r="P379">
         <v>34</v>
+      </c>
+      <c r="Q379" s="2">
+        <v>43696</v>
       </c>
     </row>
     <row r="380">
@@ -23112,6 +24252,9 @@
       <c r="P380">
         <v>34</v>
       </c>
+      <c r="Q380" s="2">
+        <v>43696</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>